<commit_message>
Created a way of getting specs for each department.
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="310">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -903,6 +903,9 @@
   </si>
   <si>
     <t xml:space="preserve">Faculty Personel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1(A)(5)(T)</t>
   </si>
   <si>
     <t xml:space="preserve">1(A)(2)(T)</t>
@@ -1100,35 +1103,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4037037037037"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.262962962963"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="3.23333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.38888888888889"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.48888888888889"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.5222222222222"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="2.35185185185185"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.38888888888889"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="37.7259259259259"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="6.85925925925926"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="6.85925925925926"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.48888888888889"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="38.6111111111111"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="7.05555555555556"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.05555555555556"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7354,13 +7357,13 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="76.4555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.3962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7575,16 +7578,16 @@
         <v>294</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>289</v>
@@ -7629,7 +7632,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -7639,7 +7642,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H11" s="5" t="n">
         <v>3</v>
@@ -7651,7 +7654,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -7661,7 +7664,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H12" s="5" t="n">
         <v>3</v>
@@ -7673,7 +7676,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -7683,7 +7686,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H13" s="5" t="n">
         <v>3</v>
@@ -7713,7 +7716,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H14" s="5" t="n">
         <v>3</v>
@@ -7725,7 +7728,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -7735,7 +7738,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H15" s="5" t="n">
         <v>3</v>
@@ -7761,7 +7764,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -7777,7 +7780,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -7793,7 +7796,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -7809,7 +7812,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -7825,7 +7828,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -7841,7 +7844,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -7857,7 +7860,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -7873,7 +7876,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -7889,7 +7892,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>

</xml_diff>

<commit_message>
Worked on a way to add names to table
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -1103,35 +1103,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.8518518518519"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="3.23333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="5.88148148148148"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.48888888888889"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="5.97777777777778"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.58518518518519"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.9111111111111"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="2.35185185185185"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="5.88148148148148"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.48888888888889"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="38.6111111111111"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="7.05555555555556"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.05555555555556"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="5.97777777777778"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.58518518518519"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="39.5888888888889"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.84074074074074"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="7.25185185185185"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="7.84074074074074"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.25185185185185"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="7.84074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7357,13 +7357,13 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="78.3962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="80.3555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added a lot of comments
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="CoC with simplified tenure trac" sheetId="1" state="visible" r:id="rId2"/>
@@ -1097,41 +1097,41 @@
   </sheetPr>
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H99" activeCellId="0" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9925925925926"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.3444444444444"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="3.23333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="5.97777777777778"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.58518518518519"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.07407407407407"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.68518518518519"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.3037037037037"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="2.35185185185185"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="5.97777777777778"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.58518518518519"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.8"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="39.5888888888889"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="7.25185185185185"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.25185185185185"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="6.07407407407407"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.68518518518519"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="40.5703703703704"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.93703703703704"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="7.34814814814815"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="7.93703703703704"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.34814814814815"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="7.93703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7356,14 +7356,14 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="80.3555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="82.4111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added Committee Constants. Fixed Drop down.
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -1097,41 +1097,40 @@
   </sheetPr>
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H99" activeCellId="0" sqref="H99"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M88" activeCellId="0" sqref="M88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3851851851852"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.8"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.8333333333333"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="3.23333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.07407407407407"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.68518518518519"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.17407407407407"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.78148148148148"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.7962962962963"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="2.35185185185185"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="6.07407407407407"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.68518518518519"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="40.5703703703704"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.93703703703704"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="7.93703703703704"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="7.93703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="6.17407407407407"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.78148148148148"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="41.6481481481481"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="8.03703703703704"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="7.44814814814815"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="8.03703703703704"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.44814814814815"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="8.03703703703704"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7362,8 +7361,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="82.4111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="84.4703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added function to FileManipulator that allows you to edit sheet to have an entire row changed. Added a way to save changed inside of CommitteeGUI. And a way to catch window close event
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -2,16 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
+  <workbookPr backupFile="false" date1904="true" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="992" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="CoC with simplified tenure trac" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CoC Specs" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CoC with simplified tenure trac" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="CoC Specs" r:id="rId3" sheetId="2" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -1016,7 +1016,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -1025,67 +1025,67 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -1097,43 +1097,43 @@
   </sheetPr>
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M88" activeCellId="0" sqref="M88"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="M88" activeCellId="0" pane="topLeft" sqref="M88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="3.23333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.17407407407407"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="2.35185185185185"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="6.17407407407407"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="41.6481481481481"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="8.03703703703704"/>
+    <col min="1" max="1" hidden="false" style="0" width="12.837037037037" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="15.3851851851852" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="1" width="3.33333333333333" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="1" width="13.1296296296296" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="1" width="9.9962962962963" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="17.2481481481481" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="18.5222222222222" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="1" width="22.8333333333333" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="1" width="3.23333333333333" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
+    <col min="12" max="12" hidden="false" style="1" width="6.17407407407407" collapsed="true"/>
+    <col min="13" max="13" hidden="false" style="1" width="5.78148148148148" collapsed="true"/>
+    <col min="14" max="14" hidden="false" style="1" width="19.7962962962963" collapsed="true"/>
+    <col min="15" max="15" hidden="false" style="1" width="2.35185185185185" collapsed="true"/>
+    <col min="16" max="16" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
+    <col min="17" max="17" hidden="false" style="1" width="6.17407407407407" collapsed="true"/>
+    <col min="18" max="18" hidden="false" style="1" width="5.78148148148148" collapsed="true"/>
+    <col min="19" max="19" hidden="false" style="1" width="10.1925925925926" collapsed="true"/>
+    <col min="20" max="20" hidden="false" style="1" width="16.2666666666667" collapsed="true"/>
+    <col min="21" max="21" hidden="false" style="1" width="26.7518518518519" collapsed="true"/>
+    <col min="22" max="22" hidden="false" style="0" width="41.6481481481481" collapsed="true"/>
+    <col min="23" max="23" hidden="false" style="0" width="30.7703703703704" collapsed="true"/>
+    <col min="24" max="24" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
+    <col min="25" max="25" hidden="false" style="1" width="7.44814814814815" collapsed="true"/>
+    <col min="26" max="26" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
+    <col min="27" max="27" hidden="false" style="1" width="7.44814814814815" collapsed="true"/>
+    <col min="28" max="28" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1" s="4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1221,7 @@
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="5" t="s">
         <v>40</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="5" t="s">
         <v>45</v>
       </c>
@@ -1453,7 +1453,7 @@
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -1517,7 +1517,7 @@
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
@@ -1589,7 +1589,7 @@
       <c r="AC7" s="5"/>
       <c r="AD7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="5" t="s">
         <v>62</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="AC8" s="5"/>
       <c r="AD8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="5" t="s">
         <v>66</v>
       </c>
@@ -1697,7 +1697,7 @@
       <c r="AC9" s="5"/>
       <c r="AD9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="5" t="s">
         <v>70</v>
       </c>
@@ -1759,7 +1759,7 @@
       <c r="AC10" s="5"/>
       <c r="AD10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="5" t="s">
         <v>74</v>
       </c>
@@ -1813,7 +1813,7 @@
       <c r="AC11" s="5"/>
       <c r="AD11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="5" t="s">
         <v>79</v>
       </c>
@@ -1875,7 +1875,7 @@
       <c r="AC12" s="5"/>
       <c r="AD12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="5" t="s">
         <v>82</v>
       </c>
@@ -1947,7 +1947,7 @@
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
@@ -2019,7 +2019,7 @@
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="5" t="s">
         <v>89</v>
       </c>
@@ -2073,7 +2073,7 @@
       <c r="AC15" s="5"/>
       <c r="AD15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="5" t="s">
         <v>94</v>
       </c>
@@ -2127,7 +2127,7 @@
       <c r="AC16" s="5"/>
       <c r="AD16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="5" t="s">
         <v>97</v>
       </c>
@@ -2179,7 +2179,7 @@
       <c r="AC17" s="5"/>
       <c r="AD17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="5" t="s">
         <v>99</v>
       </c>
@@ -2251,7 +2251,7 @@
       <c r="AC18" s="5"/>
       <c r="AD18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="5" t="s">
         <v>104</v>
       </c>
@@ -2309,7 +2309,7 @@
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="5" t="s">
         <v>107</v>
       </c>
@@ -2381,7 +2381,7 @@
       <c r="AC20" s="5"/>
       <c r="AD20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="5" t="s">
         <v>109</v>
       </c>
@@ -2433,7 +2433,7 @@
       <c r="AC21" s="5"/>
       <c r="AD21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="5" t="s">
         <v>116</v>
       </c>
@@ -2487,7 +2487,7 @@
       <c r="AC22" s="5"/>
       <c r="AD22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="5" t="s">
         <v>118</v>
       </c>
@@ -2559,7 +2559,7 @@
       <c r="AC23" s="5"/>
       <c r="AD23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
@@ -2623,7 +2623,7 @@
       <c r="AC24" s="5"/>
       <c r="AD24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="5" t="s">
         <v>125</v>
       </c>
@@ -2701,7 +2701,7 @@
       <c r="AC25" s="5"/>
       <c r="AD25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="5" t="s">
         <v>107</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="AC26" s="5"/>
       <c r="AD26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="5" t="s">
         <v>131</v>
       </c>
@@ -2815,7 +2815,7 @@
       <c r="AC27" s="5"/>
       <c r="AD27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="5" t="s">
         <v>134</v>
       </c>
@@ -2879,7 +2879,7 @@
       <c r="AC28" s="5"/>
       <c r="AD28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="A29" s="5" t="s">
         <v>136</v>
       </c>
@@ -2951,7 +2951,7 @@
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="5" t="s">
         <v>138</v>
       </c>
@@ -3013,7 +3013,7 @@
       <c r="AC30" s="5"/>
       <c r="AD30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="A31" s="5" t="s">
         <v>140</v>
       </c>
@@ -3077,7 +3077,7 @@
       <c r="AC31" s="5"/>
       <c r="AD31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="A32" s="5" t="s">
         <v>143</v>
       </c>
@@ -3149,7 +3149,7 @@
       <c r="AC32" s="5"/>
       <c r="AD32" s="5"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="5" t="s">
         <v>145</v>
       </c>
@@ -3201,7 +3201,7 @@
       <c r="AC33" s="5"/>
       <c r="AD33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="5" t="s">
         <v>149</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="AC34" s="5"/>
       <c r="AD34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="5" t="s">
         <v>151</v>
       </c>
@@ -3345,7 +3345,7 @@
       <c r="AC35" s="5"/>
       <c r="AD35" s="5"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="5" t="s">
         <v>153</v>
       </c>
@@ -3417,7 +3417,7 @@
       <c r="AC36" s="5"/>
       <c r="AD36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="5" t="s">
         <v>155</v>
       </c>
@@ -3485,7 +3485,7 @@
       <c r="AC37" s="5"/>
       <c r="AD37" s="5"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="5" t="s">
         <v>157</v>
       </c>
@@ -3557,7 +3557,7 @@
       <c r="AC38" s="5"/>
       <c r="AD38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="5" t="s">
         <v>159</v>
       </c>
@@ -3619,7 +3619,7 @@
       <c r="AC39" s="5"/>
       <c r="AD39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="5" t="s">
         <v>161</v>
       </c>
@@ -3671,7 +3671,7 @@
       <c r="AC40" s="5"/>
       <c r="AD40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="5" t="s">
         <v>163</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="AC41" s="5"/>
       <c r="AD41" s="5"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="5" t="s">
         <v>166</v>
       </c>
@@ -3805,7 +3805,7 @@
       <c r="AC42" s="5"/>
       <c r="AD42" s="5"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="5" t="s">
         <v>168</v>
       </c>
@@ -3867,7 +3867,7 @@
       <c r="AC43" s="5"/>
       <c r="AD43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="5" t="s">
         <v>170</v>
       </c>
@@ -3929,7 +3929,7 @@
       <c r="AC44" s="5"/>
       <c r="AD44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="5" t="s">
         <v>172</v>
       </c>
@@ -4001,7 +4001,7 @@
       <c r="AC45" s="5"/>
       <c r="AD45" s="5"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="5" t="s">
         <v>174</v>
       </c>
@@ -4059,7 +4059,7 @@
       <c r="AC46" s="5"/>
       <c r="AD46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="5" t="s">
         <v>176</v>
       </c>
@@ -4111,7 +4111,7 @@
       <c r="AC47" s="5"/>
       <c r="AD47" s="5"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="48">
       <c r="A48" s="5" t="s">
         <v>178</v>
       </c>
@@ -4173,7 +4173,7 @@
       <c r="AC48" s="5"/>
       <c r="AD48" s="5"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="49">
       <c r="A49" s="5" t="s">
         <v>180</v>
       </c>
@@ -4235,7 +4235,7 @@
       <c r="AC49" s="5"/>
       <c r="AD49" s="5"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="A50" s="5" t="s">
         <v>182</v>
       </c>
@@ -4307,7 +4307,7 @@
       <c r="AC50" s="5"/>
       <c r="AD50" s="5"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="51">
       <c r="A51" s="5" t="s">
         <v>184</v>
       </c>
@@ -4379,7 +4379,7 @@
       <c r="AC51" s="5"/>
       <c r="AD51" s="5"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="52">
       <c r="A52" s="5" t="s">
         <v>140</v>
       </c>
@@ -4447,7 +4447,7 @@
       <c r="AC52" s="5"/>
       <c r="AD52" s="5"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="A53" s="5" t="s">
         <v>188</v>
       </c>
@@ -4509,7 +4509,7 @@
       <c r="AC53" s="5"/>
       <c r="AD53" s="5"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="54">
       <c r="A54" s="5" t="s">
         <v>62</v>
       </c>
@@ -4581,7 +4581,7 @@
       <c r="AC54" s="5"/>
       <c r="AD54" s="5"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="55">
       <c r="A55" s="5" t="s">
         <v>191</v>
       </c>
@@ -4643,7 +4643,7 @@
       <c r="AC55" s="5"/>
       <c r="AD55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="56">
       <c r="A56" s="5" t="s">
         <v>192</v>
       </c>
@@ -4695,7 +4695,7 @@
       <c r="AC56" s="5"/>
       <c r="AD56" s="5"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="57">
       <c r="A57" s="5" t="s">
         <v>195</v>
       </c>
@@ -4767,7 +4767,7 @@
       <c r="AC57" s="5"/>
       <c r="AD57" s="5"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="58">
       <c r="A58" s="5" t="s">
         <v>198</v>
       </c>
@@ -4819,7 +4819,7 @@
       <c r="AC58" s="5"/>
       <c r="AD58" s="5"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="59">
       <c r="A59" s="5" t="s">
         <v>138</v>
       </c>
@@ -4891,7 +4891,7 @@
       <c r="AC59" s="5"/>
       <c r="AD59" s="5"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="60">
       <c r="A60" s="5" t="s">
         <v>202</v>
       </c>
@@ -4951,7 +4951,7 @@
       <c r="AC60" s="5"/>
       <c r="AD60" s="5"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="61">
       <c r="A61" s="5" t="s">
         <v>205</v>
       </c>
@@ -5023,7 +5023,7 @@
       <c r="AC61" s="5"/>
       <c r="AD61" s="5"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="62">
       <c r="A62" s="5" t="s">
         <v>207</v>
       </c>
@@ -5085,7 +5085,7 @@
       <c r="AC62" s="5"/>
       <c r="AD62" s="5"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="63">
       <c r="A63" s="5" t="s">
         <v>209</v>
       </c>
@@ -5157,7 +5157,7 @@
       <c r="AC63" s="5"/>
       <c r="AD63" s="5"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="64">
       <c r="A64" s="5" t="s">
         <v>211</v>
       </c>
@@ -5209,7 +5209,7 @@
       <c r="AC64" s="5"/>
       <c r="AD64" s="5"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="65">
       <c r="A65" s="5" t="s">
         <v>213</v>
       </c>
@@ -5281,7 +5281,7 @@
       <c r="AC65" s="5"/>
       <c r="AD65" s="5"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="66">
       <c r="A66" s="5" t="s">
         <v>215</v>
       </c>
@@ -5353,7 +5353,7 @@
       <c r="AC66" s="5"/>
       <c r="AD66" s="5"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="67">
       <c r="A67" s="5" t="s">
         <v>217</v>
       </c>
@@ -5415,7 +5415,7 @@
       <c r="AC67" s="5"/>
       <c r="AD67" s="5"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="68">
       <c r="A68" s="5" t="s">
         <v>62</v>
       </c>
@@ -5487,7 +5487,7 @@
       <c r="AC68" s="5"/>
       <c r="AD68" s="5"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="69">
       <c r="A69" s="5" t="s">
         <v>221</v>
       </c>
@@ -5539,7 +5539,7 @@
       <c r="AC69" s="5"/>
       <c r="AD69" s="5"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="70">
       <c r="A70" s="5" t="s">
         <v>223</v>
       </c>
@@ -5591,7 +5591,7 @@
       <c r="AC70" s="5"/>
       <c r="AD70" s="5"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="A71" s="5" t="s">
         <v>225</v>
       </c>
@@ -5669,7 +5669,7 @@
       <c r="AC71" s="5"/>
       <c r="AD71" s="5"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="72">
       <c r="A72" s="5" t="s">
         <v>227</v>
       </c>
@@ -5723,7 +5723,7 @@
       <c r="AC72" s="5"/>
       <c r="AD72" s="5"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="73">
       <c r="A73" s="5" t="s">
         <v>47</v>
       </c>
@@ -5795,7 +5795,7 @@
       <c r="AC73" s="5"/>
       <c r="AD73" s="5"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="74">
       <c r="A74" s="5" t="s">
         <v>233</v>
       </c>
@@ -5867,7 +5867,7 @@
       <c r="AC74" s="5"/>
       <c r="AD74" s="5"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="75">
       <c r="A75" s="5" t="s">
         <v>178</v>
       </c>
@@ -5939,7 +5939,7 @@
       <c r="AC75" s="5"/>
       <c r="AD75" s="5"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="76">
       <c r="A76" s="5" t="s">
         <v>82</v>
       </c>
@@ -5991,7 +5991,7 @@
       <c r="AC76" s="5"/>
       <c r="AD76" s="5"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="77">
       <c r="A77" s="5" t="s">
         <v>237</v>
       </c>
@@ -6043,7 +6043,7 @@
       <c r="AC77" s="5"/>
       <c r="AD77" s="5"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="78">
       <c r="A78" s="5" t="s">
         <v>239</v>
       </c>
@@ -6095,7 +6095,7 @@
       <c r="AC78" s="5"/>
       <c r="AD78" s="5"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="79">
       <c r="A79" s="5" t="s">
         <v>241</v>
       </c>
@@ -6147,7 +6147,7 @@
       <c r="AC79" s="5"/>
       <c r="AD79" s="5"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="80">
       <c r="A80" s="5" t="s">
         <v>62</v>
       </c>
@@ -6209,7 +6209,7 @@
       <c r="AC80" s="5"/>
       <c r="AD80" s="5"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="81">
       <c r="A81" s="5" t="s">
         <v>244</v>
       </c>
@@ -6281,7 +6281,7 @@
       <c r="AC81" s="5"/>
       <c r="AD81" s="5"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="82">
       <c r="A82" s="5" t="s">
         <v>245</v>
       </c>
@@ -6333,7 +6333,7 @@
       <c r="AC82" s="5"/>
       <c r="AD82" s="5"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="83">
       <c r="A83" s="5" t="s">
         <v>247</v>
       </c>
@@ -6395,7 +6395,7 @@
       <c r="AC83" s="5"/>
       <c r="AD83" s="5"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="84">
       <c r="A84" s="5" t="s">
         <v>249</v>
       </c>
@@ -6447,7 +6447,7 @@
       <c r="AC84" s="5"/>
       <c r="AD84" s="5"/>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="85">
       <c r="A85" s="5" t="s">
         <v>168</v>
       </c>
@@ -6509,7 +6509,7 @@
       <c r="AC85" s="5"/>
       <c r="AD85" s="5"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="86">
       <c r="A86" s="5" t="s">
         <v>253</v>
       </c>
@@ -6581,7 +6581,7 @@
       <c r="AC86" s="5"/>
       <c r="AD86" s="5"/>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="87">
       <c r="A87" s="5" t="s">
         <v>256</v>
       </c>
@@ -6653,7 +6653,7 @@
       <c r="AC87" s="5"/>
       <c r="AD87" s="5"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="88">
       <c r="A88" s="5" t="s">
         <v>258</v>
       </c>
@@ -6715,7 +6715,7 @@
       <c r="AC88" s="5"/>
       <c r="AD88" s="5"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="89">
       <c r="A89" s="5" t="s">
         <v>260</v>
       </c>
@@ -6777,7 +6777,7 @@
       <c r="AC89" s="5"/>
       <c r="AD89" s="5"/>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="90">
       <c r="A90" s="5" t="s">
         <v>262</v>
       </c>
@@ -6829,7 +6829,7 @@
       <c r="AC90" s="5"/>
       <c r="AD90" s="5"/>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="91">
       <c r="A91" s="5" t="s">
         <v>205</v>
       </c>
@@ -6881,7 +6881,7 @@
       <c r="AC91" s="5"/>
       <c r="AD91" s="5"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="92">
       <c r="A92" s="5" t="s">
         <v>266</v>
       </c>
@@ -6943,7 +6943,7 @@
       <c r="AC92" s="5"/>
       <c r="AD92" s="5"/>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="93">
       <c r="A93" s="5" t="s">
         <v>268</v>
       </c>
@@ -6995,7 +6995,7 @@
       <c r="AC93" s="5"/>
       <c r="AD93" s="5"/>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="94">
       <c r="A94" s="5" t="s">
         <v>25</v>
       </c>
@@ -7057,7 +7057,7 @@
       <c r="AC94" s="5"/>
       <c r="AD94" s="5"/>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="95">
       <c r="A95" s="5" t="s">
         <v>271</v>
       </c>
@@ -7109,7 +7109,7 @@
       <c r="AC95" s="5"/>
       <c r="AD95" s="5"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="96">
       <c r="A96" s="5" t="s">
         <v>273</v>
       </c>
@@ -7171,7 +7171,7 @@
       <c r="AC96" s="5"/>
       <c r="AD96" s="5"/>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="97">
       <c r="A97" s="5" t="s">
         <v>275</v>
       </c>
@@ -7233,7 +7233,7 @@
       <c r="AC97" s="5"/>
       <c r="AD97" s="5"/>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="98">
       <c r="A98" s="5" t="s">
         <v>277</v>
       </c>
@@ -7285,7 +7285,7 @@
       <c r="AC98" s="5"/>
       <c r="AD98" s="5"/>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="99">
       <c r="A99" s="5" t="s">
         <v>178</v>
       </c>
@@ -7338,9 +7338,9 @@
       <c r="AD99" s="5"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7355,17 +7355,17 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="H9" activeCellId="0" pane="topLeft" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="84.4703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.01481481481481"/>
+    <col min="1" max="1" hidden="false" style="0" width="84.4703703703704" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="9.01481481481481" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="5" t="s">
         <v>280</v>
       </c>
@@ -7387,7 +7387,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
         <v>284</v>
@@ -7409,7 +7409,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="5" t="s">
         <v>288</v>
       </c>
@@ -7435,7 +7435,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -7449,7 +7449,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -7479,7 +7479,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
@@ -7509,7 +7509,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="5" t="s">
         <v>290</v>
       </c>
@@ -7539,7 +7539,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -7569,7 +7569,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="5" t="s">
         <v>293</v>
       </c>
@@ -7599,7 +7599,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="5" t="s">
         <v>81</v>
       </c>
@@ -7629,7 +7629,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="5" t="s">
         <v>296</v>
       </c>
@@ -7651,7 +7651,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="5" t="s">
         <v>298</v>
       </c>
@@ -7673,7 +7673,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="5" t="s">
         <v>299</v>
       </c>
@@ -7695,7 +7695,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="5" t="s">
         <v>59</v>
       </c>
@@ -7725,7 +7725,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="5" t="s">
         <v>300</v>
       </c>
@@ -7747,7 +7747,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -7761,7 +7761,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="5" t="s">
         <v>301</v>
       </c>
@@ -7777,7 +7777,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="5" t="s">
         <v>302</v>
       </c>
@@ -7793,7 +7793,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="5" t="s">
         <v>303</v>
       </c>
@@ -7809,7 +7809,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="5" t="s">
         <v>304</v>
       </c>
@@ -7825,7 +7825,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="5" t="s">
         <v>305</v>
       </c>
@@ -7841,7 +7841,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="5" t="s">
         <v>306</v>
       </c>
@@ -7857,7 +7857,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="5" t="s">
         <v>307</v>
       </c>
@@ -7873,7 +7873,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="5" t="s">
         <v>308</v>
       </c>
@@ -7889,7 +7889,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="5" t="s">
         <v>309</v>
       </c>
@@ -7906,9 +7906,9 @@
       <c r="L25" s="5"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Able to save now. I need to figure out a way to update all of the worksheets now though
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="323">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -951,6 +951,45 @@
   </si>
   <si>
     <t xml:space="preserve">FacChair is not elegible for election or appointment to a committee</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Pullum</t>
+  </si>
+  <si>
+    <t>HSS</t>
+  </si>
+  <si>
+    <t>Lang &amp; Literature</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>AASFA</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>VALC</t>
+  </si>
+  <si>
+    <t>FERC</t>
+  </si>
+  <si>
+    <t>Lib</t>
   </si>
 </sst>
 </file>
@@ -1095,42 +1134,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD99"/>
+  <dimension ref="1:99"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="M88" activeCellId="0" pane="topLeft" sqref="M88"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="AC49" activeCellId="0" pane="topLeft" sqref="AC49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="12.837037037037" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="15.3851851851852" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="13.4259259259259" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="16.1703703703704" collapsed="true"/>
     <col min="3" max="3" hidden="false" style="1" width="3.33333333333333" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="1" width="13.1296296296296" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="1" width="9.9962962962963" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="17.2481481481481" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="18.5222222222222" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="1" width="22.8333333333333" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="1" width="13.7185185185185" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="1" width="10.3888888888889" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="18.0296296296296" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="19.3037037037037" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="1" width="16.462962962963" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="1" width="23.8111111111111" collapsed="true"/>
     <col min="10" max="10" hidden="false" style="1" width="3.23333333333333" collapsed="true"/>
-    <col min="11" max="11" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
-    <col min="12" max="12" hidden="false" style="1" width="6.17407407407407" collapsed="true"/>
-    <col min="13" max="13" hidden="false" style="1" width="5.78148148148148" collapsed="true"/>
-    <col min="14" max="14" hidden="false" style="1" width="19.7962962962963" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="1" width="16.462962962963" collapsed="true"/>
+    <col min="12" max="12" hidden="false" style="1" width="6.37037037037037" collapsed="true"/>
+    <col min="13" max="13" hidden="false" style="1" width="5.97777777777778" collapsed="true"/>
+    <col min="14" max="14" hidden="false" style="1" width="20.7740740740741" collapsed="true"/>
     <col min="15" max="15" hidden="false" style="1" width="2.35185185185185" collapsed="true"/>
-    <col min="16" max="16" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
-    <col min="17" max="17" hidden="false" style="1" width="6.17407407407407" collapsed="true"/>
-    <col min="18" max="18" hidden="false" style="1" width="5.78148148148148" collapsed="true"/>
-    <col min="19" max="19" hidden="false" style="1" width="10.1925925925926" collapsed="true"/>
-    <col min="20" max="20" hidden="false" style="1" width="16.2666666666667" collapsed="true"/>
-    <col min="21" max="21" hidden="false" style="1" width="26.7518518518519" collapsed="true"/>
-    <col min="22" max="22" hidden="false" style="0" width="41.6481481481481" collapsed="true"/>
-    <col min="23" max="23" hidden="false" style="0" width="30.7703703703704" collapsed="true"/>
-    <col min="24" max="24" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
-    <col min="25" max="25" hidden="false" style="1" width="7.44814814814815" collapsed="true"/>
-    <col min="26" max="26" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
-    <col min="27" max="27" hidden="false" style="1" width="7.44814814814815" collapsed="true"/>
-    <col min="28" max="28" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
+    <col min="16" max="16" hidden="false" style="1" width="16.462962962963" collapsed="true"/>
+    <col min="17" max="17" hidden="false" style="1" width="6.37037037037037" collapsed="true"/>
+    <col min="18" max="18" hidden="false" style="1" width="5.97777777777778" collapsed="true"/>
+    <col min="19" max="19" hidden="false" style="1" width="10.5851851851852" collapsed="true"/>
+    <col min="20" max="20" hidden="false" style="1" width="17.0518518518519" collapsed="true"/>
+    <col min="21" max="21" hidden="false" style="1" width="27.9296296296296" collapsed="true"/>
+    <col min="22" max="22" hidden="false" style="0" width="43.7037037037037" collapsed="true"/>
+    <col min="23" max="23" hidden="false" style="0" width="32.337037037037" collapsed="true"/>
+    <col min="24" max="24" hidden="false" style="1" width="8.23333333333333" collapsed="true"/>
+    <col min="25" max="25" hidden="false" style="1" width="7.64444444444445" collapsed="true"/>
+    <col min="26" max="26" hidden="false" style="1" width="8.23333333333333" collapsed="true"/>
+    <col min="27" max="27" hidden="false" style="1" width="7.64444444444445" collapsed="true"/>
+    <col min="28" max="28" hidden="false" style="1" width="8.23333333333333" collapsed="true"/>
+    <col min="29" max="1025" hidden="false" style="0" width="8.81851851851852" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1" s="4">
@@ -1218,8 +1258,8 @@
       <c r="AB1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="5" t="s">
@@ -1270,8 +1310,6 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="5" t="s">
@@ -1332,8 +1370,6 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="5" t="s">
@@ -1394,8 +1430,6 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="5" t="s">
@@ -1450,8 +1484,6 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="5" t="s">
@@ -1514,46 +1546,44 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="5" t="s">
-        <v>53</v>
+        <v>310</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>54</v>
+        <v>311</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>6</v>
+        <v>6.0</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>55</v>
+        <v>312</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>56</v>
+        <v>313</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>57</v>
+        <v>314</v>
       </c>
       <c r="H7" s="6" t="n">
-        <v>1990</v>
+        <v>1990.0</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>58</v>
+        <v>315</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>38</v>
+        <v>316</v>
       </c>
       <c r="L7" s="6" t="n">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>39</v>
+        <v>317</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -1561,33 +1591,31 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="6" t="s">
-        <v>30</v>
+        <v>318</v>
       </c>
       <c r="T7" s="6" t="n">
-        <v>1996</v>
+        <v>1996.0</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="6" t="s">
-        <v>59</v>
+        <v>320</v>
       </c>
       <c r="Y7" s="6" t="s">
-        <v>44</v>
+        <v>321</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>60</v>
+        <v>322</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>58</v>
+        <v>315</v>
       </c>
       <c r="AB7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="5" t="s">
@@ -1640,8 +1668,6 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="5" t="s">
@@ -1694,8 +1720,6 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="5" t="s">
@@ -1756,8 +1780,6 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="5" t="s">
@@ -1810,8 +1832,6 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="5" t="s">
@@ -1872,8 +1892,6 @@
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="5" t="s">
@@ -1944,8 +1962,6 @@
       <c r="AB13" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="5" t="s">
@@ -2016,8 +2032,6 @@
       <c r="AB14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="5" t="s">
@@ -2070,8 +2084,6 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
-      <c r="AC15" s="5"/>
-      <c r="AD15" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="5" t="s">
@@ -2124,8 +2136,6 @@
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
-      <c r="AC16" s="5"/>
-      <c r="AD16" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="5" t="s">
@@ -2176,8 +2186,6 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="5" t="s">
@@ -2248,8 +2256,6 @@
       <c r="AB18" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AC18" s="5"/>
-      <c r="AD18" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="5" t="s">
@@ -2306,8 +2312,6 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
-      <c r="AC19" s="5"/>
-      <c r="AD19" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="5" t="s">
@@ -2378,8 +2382,6 @@
       <c r="AB20" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AC20" s="5"/>
-      <c r="AD20" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="5" t="s">
@@ -2430,8 +2432,6 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
       <c r="AB21" s="5"/>
-      <c r="AC21" s="5"/>
-      <c r="AD21" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="5" t="s">
@@ -2484,8 +2484,6 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
-      <c r="AC22" s="5"/>
-      <c r="AD22" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="5" t="s">
@@ -2556,8 +2554,6 @@
       <c r="AB23" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="AC23" s="5"/>
-      <c r="AD23" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="5" t="s">
@@ -2620,8 +2616,6 @@
       <c r="AB24" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="5" t="s">
@@ -2698,8 +2692,6 @@
       <c r="AB25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC25" s="5"/>
-      <c r="AD25" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="5" t="s">
@@ -2758,8 +2750,6 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
-      <c r="AC26" s="5"/>
-      <c r="AD26" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="5" t="s">
@@ -2812,8 +2802,6 @@
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
       <c r="AB27" s="5"/>
-      <c r="AC27" s="5"/>
-      <c r="AD27" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="5" t="s">
@@ -2876,8 +2864,6 @@
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="A29" s="5" t="s">
@@ -2948,8 +2934,6 @@
       <c r="AB29" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="5" t="s">
@@ -3010,8 +2994,6 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
       <c r="AB30" s="5"/>
-      <c r="AC30" s="5"/>
-      <c r="AD30" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="A31" s="5" t="s">
@@ -3074,8 +3056,6 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="5"/>
       <c r="AB31" s="5"/>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="A32" s="5" t="s">
@@ -3146,8 +3126,6 @@
       <c r="AB32" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="5" t="s">
@@ -3198,8 +3176,6 @@
       <c r="Z33" s="5"/>
       <c r="AA33" s="5"/>
       <c r="AB33" s="5"/>
-      <c r="AC33" s="5"/>
-      <c r="AD33" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="5" t="s">
@@ -3270,8 +3246,6 @@
       <c r="AB34" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AC34" s="5"/>
-      <c r="AD34" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="5" t="s">
@@ -3342,8 +3316,6 @@
       <c r="AB35" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AC35" s="5"/>
-      <c r="AD35" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="5" t="s">
@@ -3414,8 +3386,6 @@
       <c r="AB36" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AC36" s="5"/>
-      <c r="AD36" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="5" t="s">
@@ -3482,8 +3452,6 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
       <c r="AB37" s="5"/>
-      <c r="AC37" s="5"/>
-      <c r="AD37" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="5" t="s">
@@ -3554,8 +3522,6 @@
       <c r="AB38" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AC38" s="5"/>
-      <c r="AD38" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="5" t="s">
@@ -3616,8 +3582,6 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
       <c r="AB39" s="5"/>
-      <c r="AC39" s="5"/>
-      <c r="AD39" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="5" t="s">
@@ -3668,8 +3632,6 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
       <c r="AB40" s="5"/>
-      <c r="AC40" s="5"/>
-      <c r="AD40" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="5" t="s">
@@ -3730,8 +3692,6 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="5"/>
       <c r="AB41" s="5"/>
-      <c r="AC41" s="5"/>
-      <c r="AD41" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="5" t="s">
@@ -3802,8 +3762,6 @@
       <c r="AB42" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AC42" s="5"/>
-      <c r="AD42" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="5" t="s">
@@ -3864,8 +3822,6 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
       <c r="AB43" s="5"/>
-      <c r="AC43" s="5"/>
-      <c r="AD43" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="5" t="s">
@@ -3926,8 +3882,6 @@
       <c r="AB44" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC44" s="5"/>
-      <c r="AD44" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="5" t="s">
@@ -3998,8 +3952,6 @@
       <c r="AB45" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AC45" s="5"/>
-      <c r="AD45" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="5" t="s">
@@ -4056,8 +4008,6 @@
       </c>
       <c r="AA46" s="5"/>
       <c r="AB46" s="5"/>
-      <c r="AC46" s="5"/>
-      <c r="AD46" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="5" t="s">
@@ -4108,8 +4058,6 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
       <c r="AB47" s="5"/>
-      <c r="AC47" s="5"/>
-      <c r="AD47" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="48">
       <c r="A48" s="5" t="s">
@@ -4170,8 +4118,6 @@
       <c r="AB48" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AC48" s="5"/>
-      <c r="AD48" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="49">
       <c r="A49" s="5" t="s">
@@ -4232,8 +4178,6 @@
       <c r="Z49" s="5"/>
       <c r="AA49" s="5"/>
       <c r="AB49" s="5"/>
-      <c r="AC49" s="5"/>
-      <c r="AD49" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="A50" s="5" t="s">
@@ -4304,8 +4248,6 @@
       <c r="AB50" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AC50" s="5"/>
-      <c r="AD50" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="51">
       <c r="A51" s="5" t="s">
@@ -4376,8 +4318,6 @@
       <c r="AB51" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AC51" s="5"/>
-      <c r="AD51" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="52">
       <c r="A52" s="5" t="s">
@@ -4444,8 +4384,6 @@
       <c r="Z52" s="5"/>
       <c r="AA52" s="5"/>
       <c r="AB52" s="5"/>
-      <c r="AC52" s="5"/>
-      <c r="AD52" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="A53" s="5" t="s">
@@ -4506,8 +4444,6 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
       <c r="AB53" s="5"/>
-      <c r="AC53" s="5"/>
-      <c r="AD53" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="54">
       <c r="A54" s="5" t="s">
@@ -4578,8 +4514,6 @@
       <c r="AB54" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AC54" s="5"/>
-      <c r="AD54" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="55">
       <c r="A55" s="5" t="s">
@@ -4640,8 +4574,6 @@
       <c r="Z55" s="5"/>
       <c r="AA55" s="5"/>
       <c r="AB55" s="5"/>
-      <c r="AC55" s="5"/>
-      <c r="AD55" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="56">
       <c r="A56" s="5" t="s">
@@ -4692,8 +4624,6 @@
       <c r="Z56" s="5"/>
       <c r="AA56" s="5"/>
       <c r="AB56" s="5"/>
-      <c r="AC56" s="5"/>
-      <c r="AD56" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="57">
       <c r="A57" s="5" t="s">
@@ -4764,8 +4694,6 @@
       <c r="AB57" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC57" s="5"/>
-      <c r="AD57" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="58">
       <c r="A58" s="5" t="s">
@@ -4816,8 +4744,6 @@
       <c r="Z58" s="5"/>
       <c r="AA58" s="5"/>
       <c r="AB58" s="5"/>
-      <c r="AC58" s="5"/>
-      <c r="AD58" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="59">
       <c r="A59" s="5" t="s">
@@ -4888,8 +4814,6 @@
       <c r="AB59" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AC59" s="5"/>
-      <c r="AD59" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="60">
       <c r="A60" s="5" t="s">
@@ -4948,8 +4872,6 @@
       <c r="Z60" s="5"/>
       <c r="AA60" s="5"/>
       <c r="AB60" s="5"/>
-      <c r="AC60" s="5"/>
-      <c r="AD60" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="61">
       <c r="A61" s="5" t="s">
@@ -5020,8 +4942,6 @@
       <c r="AB61" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AC61" s="5"/>
-      <c r="AD61" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="62">
       <c r="A62" s="5" t="s">
@@ -5082,8 +5002,6 @@
       <c r="Z62" s="5"/>
       <c r="AA62" s="5"/>
       <c r="AB62" s="5"/>
-      <c r="AC62" s="5"/>
-      <c r="AD62" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="63">
       <c r="A63" s="5" t="s">
@@ -5154,8 +5072,6 @@
       <c r="AB63" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AC63" s="5"/>
-      <c r="AD63" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="64">
       <c r="A64" s="5" t="s">
@@ -5206,8 +5122,6 @@
       <c r="Z64" s="5"/>
       <c r="AA64" s="5"/>
       <c r="AB64" s="5"/>
-      <c r="AC64" s="5"/>
-      <c r="AD64" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="65">
       <c r="A65" s="5" t="s">
@@ -5278,8 +5192,6 @@
       <c r="AB65" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AC65" s="5"/>
-      <c r="AD65" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="66">
       <c r="A66" s="5" t="s">
@@ -5350,8 +5262,6 @@
       <c r="AB66" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="AC66" s="5"/>
-      <c r="AD66" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="67">
       <c r="A67" s="5" t="s">
@@ -5412,8 +5322,6 @@
       <c r="Z67" s="5"/>
       <c r="AA67" s="5"/>
       <c r="AB67" s="5"/>
-      <c r="AC67" s="5"/>
-      <c r="AD67" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="68">
       <c r="A68" s="5" t="s">
@@ -5484,8 +5392,6 @@
       <c r="AB68" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC68" s="5"/>
-      <c r="AD68" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="69">
       <c r="A69" s="5" t="s">
@@ -5536,8 +5442,6 @@
       <c r="Z69" s="5"/>
       <c r="AA69" s="5"/>
       <c r="AB69" s="5"/>
-      <c r="AC69" s="5"/>
-      <c r="AD69" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="70">
       <c r="A70" s="5" t="s">
@@ -5588,8 +5492,6 @@
       <c r="Z70" s="5"/>
       <c r="AA70" s="5"/>
       <c r="AB70" s="5"/>
-      <c r="AC70" s="5"/>
-      <c r="AD70" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="A71" s="5" t="s">
@@ -5666,8 +5568,6 @@
       <c r="AB71" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AC71" s="5"/>
-      <c r="AD71" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="72">
       <c r="A72" s="5" t="s">
@@ -5720,8 +5620,6 @@
       <c r="Z72" s="5"/>
       <c r="AA72" s="5"/>
       <c r="AB72" s="5"/>
-      <c r="AC72" s="5"/>
-      <c r="AD72" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="73">
       <c r="A73" s="5" t="s">
@@ -5792,8 +5690,6 @@
       <c r="AB73" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="AC73" s="5"/>
-      <c r="AD73" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="74">
       <c r="A74" s="5" t="s">
@@ -5864,8 +5760,6 @@
       <c r="AB74" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="AC74" s="5"/>
-      <c r="AD74" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="75">
       <c r="A75" s="5" t="s">
@@ -5936,8 +5830,6 @@
       <c r="AB75" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AC75" s="5"/>
-      <c r="AD75" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="76">
       <c r="A76" s="5" t="s">
@@ -5988,8 +5880,6 @@
       <c r="Z76" s="5"/>
       <c r="AA76" s="5"/>
       <c r="AB76" s="5"/>
-      <c r="AC76" s="5"/>
-      <c r="AD76" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="77">
       <c r="A77" s="5" t="s">
@@ -6040,8 +5930,6 @@
       <c r="Z77" s="5"/>
       <c r="AA77" s="5"/>
       <c r="AB77" s="5"/>
-      <c r="AC77" s="5"/>
-      <c r="AD77" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="78">
       <c r="A78" s="5" t="s">
@@ -6092,8 +5980,6 @@
       <c r="Z78" s="5"/>
       <c r="AA78" s="5"/>
       <c r="AB78" s="5"/>
-      <c r="AC78" s="5"/>
-      <c r="AD78" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="79">
       <c r="A79" s="5" t="s">
@@ -6144,8 +6030,6 @@
       <c r="Z79" s="5"/>
       <c r="AA79" s="5"/>
       <c r="AB79" s="5"/>
-      <c r="AC79" s="5"/>
-      <c r="AD79" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="80">
       <c r="A80" s="5" t="s">
@@ -6206,8 +6090,6 @@
       <c r="AB80" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AC80" s="5"/>
-      <c r="AD80" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="81">
       <c r="A81" s="5" t="s">
@@ -6278,8 +6160,6 @@
       <c r="AB81" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AC81" s="5"/>
-      <c r="AD81" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="82">
       <c r="A82" s="5" t="s">
@@ -6330,8 +6210,6 @@
       <c r="Z82" s="5"/>
       <c r="AA82" s="5"/>
       <c r="AB82" s="5"/>
-      <c r="AC82" s="5"/>
-      <c r="AD82" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="83">
       <c r="A83" s="5" t="s">
@@ -6392,8 +6270,6 @@
       <c r="AB83" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC83" s="5"/>
-      <c r="AD83" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="84">
       <c r="A84" s="5" t="s">
@@ -6444,8 +6320,6 @@
       <c r="Z84" s="5"/>
       <c r="AA84" s="5"/>
       <c r="AB84" s="5"/>
-      <c r="AC84" s="5"/>
-      <c r="AD84" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="85">
       <c r="A85" s="5" t="s">
@@ -6506,8 +6380,6 @@
       <c r="Z85" s="5"/>
       <c r="AA85" s="5"/>
       <c r="AB85" s="5"/>
-      <c r="AC85" s="5"/>
-      <c r="AD85" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="86">
       <c r="A86" s="5" t="s">
@@ -6578,8 +6450,6 @@
       <c r="AB86" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AC86" s="5"/>
-      <c r="AD86" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="87">
       <c r="A87" s="5" t="s">
@@ -6650,8 +6520,6 @@
       <c r="AB87" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AC87" s="5"/>
-      <c r="AD87" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="88">
       <c r="A88" s="5" t="s">
@@ -6712,8 +6580,6 @@
       <c r="AB88" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AC88" s="5"/>
-      <c r="AD88" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="89">
       <c r="A89" s="5" t="s">
@@ -6774,8 +6640,6 @@
       <c r="AB89" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AC89" s="5"/>
-      <c r="AD89" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="90">
       <c r="A90" s="5" t="s">
@@ -6826,8 +6690,6 @@
       <c r="Z90" s="5"/>
       <c r="AA90" s="5"/>
       <c r="AB90" s="5"/>
-      <c r="AC90" s="5"/>
-      <c r="AD90" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="91">
       <c r="A91" s="5" t="s">
@@ -6878,8 +6740,6 @@
       <c r="Z91" s="5"/>
       <c r="AA91" s="5"/>
       <c r="AB91" s="5"/>
-      <c r="AC91" s="5"/>
-      <c r="AD91" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="92">
       <c r="A92" s="5" t="s">
@@ -6940,8 +6800,6 @@
       <c r="AB92" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC92" s="5"/>
-      <c r="AD92" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="93">
       <c r="A93" s="5" t="s">
@@ -6992,8 +6850,6 @@
       <c r="Z93" s="5"/>
       <c r="AA93" s="5"/>
       <c r="AB93" s="5"/>
-      <c r="AC93" s="5"/>
-      <c r="AD93" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="94">
       <c r="A94" s="5" t="s">
@@ -7054,8 +6910,6 @@
       <c r="AB94" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC94" s="5"/>
-      <c r="AD94" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="95">
       <c r="A95" s="5" t="s">
@@ -7106,8 +6960,6 @@
       <c r="Z95" s="5"/>
       <c r="AA95" s="5"/>
       <c r="AB95" s="5"/>
-      <c r="AC95" s="5"/>
-      <c r="AD95" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="96">
       <c r="A96" s="5" t="s">
@@ -7168,8 +7020,6 @@
       <c r="AB96" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AC96" s="5"/>
-      <c r="AD96" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="97">
       <c r="A97" s="5" t="s">
@@ -7230,8 +7080,6 @@
       <c r="AB97" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AC97" s="5"/>
-      <c r="AD97" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="98">
       <c r="A98" s="5" t="s">
@@ -7282,8 +7130,6 @@
       <c r="Z98" s="6"/>
       <c r="AA98" s="6"/>
       <c r="AB98" s="6"/>
-      <c r="AC98" s="5"/>
-      <c r="AD98" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="99">
       <c r="A99" s="5" t="s">
@@ -7334,8 +7180,6 @@
       <c r="Z99" s="6"/>
       <c r="AA99" s="6"/>
       <c r="AB99" s="6"/>
-      <c r="AC99" s="5"/>
-      <c r="AD99" s="5"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
@@ -7361,8 +7205,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="84.4703703703704" collapsed="true"/>
-    <col min="2" max="1025" hidden="false" style="0" width="9.01481481481481" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="88.7814814814815" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="9.40740740740741" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Made FileManip Static and corrected error where we were setting Professorsheet to something else inside of Requirements
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="310">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -951,45 +951,6 @@
   </si>
   <si>
     <t xml:space="preserve">FacChair is not elegible for election or appointment to a committee</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>Pullum</t>
-  </si>
-  <si>
-    <t>HSS</t>
-  </si>
-  <si>
-    <t>Lang &amp; Literature</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>AASFA</t>
-  </si>
-  <si>
-    <t>DIV</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Professor</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>VALC</t>
-  </si>
-  <si>
-    <t>FERC</t>
-  </si>
-  <si>
-    <t>Lib</t>
   </si>
 </sst>
 </file>
@@ -1134,43 +1095,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:99"/>
+  <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="AC49" activeCellId="0" pane="topLeft" sqref="AC49"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="M88" activeCellId="0" pane="topLeft" sqref="M88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="13.4259259259259" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="16.1703703703704" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="12.837037037037" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="15.3851851851852" collapsed="true"/>
     <col min="3" max="3" hidden="false" style="1" width="3.33333333333333" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="1" width="13.7185185185185" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="1" width="10.3888888888889" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="18.0296296296296" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="19.3037037037037" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="1" width="16.462962962963" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="1" width="23.8111111111111" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="1" width="13.1296296296296" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="1" width="9.9962962962963" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="17.2481481481481" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="18.5222222222222" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="1" width="22.8333333333333" collapsed="true"/>
     <col min="10" max="10" hidden="false" style="1" width="3.23333333333333" collapsed="true"/>
-    <col min="11" max="11" hidden="false" style="1" width="16.462962962963" collapsed="true"/>
-    <col min="12" max="12" hidden="false" style="1" width="6.37037037037037" collapsed="true"/>
-    <col min="13" max="13" hidden="false" style="1" width="5.97777777777778" collapsed="true"/>
-    <col min="14" max="14" hidden="false" style="1" width="20.7740740740741" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
+    <col min="12" max="12" hidden="false" style="1" width="6.17407407407407" collapsed="true"/>
+    <col min="13" max="13" hidden="false" style="1" width="5.78148148148148" collapsed="true"/>
+    <col min="14" max="14" hidden="false" style="1" width="19.7962962962963" collapsed="true"/>
     <col min="15" max="15" hidden="false" style="1" width="2.35185185185185" collapsed="true"/>
-    <col min="16" max="16" hidden="false" style="1" width="16.462962962963" collapsed="true"/>
-    <col min="17" max="17" hidden="false" style="1" width="6.37037037037037" collapsed="true"/>
-    <col min="18" max="18" hidden="false" style="1" width="5.97777777777778" collapsed="true"/>
-    <col min="19" max="19" hidden="false" style="1" width="10.5851851851852" collapsed="true"/>
-    <col min="20" max="20" hidden="false" style="1" width="17.0518518518519" collapsed="true"/>
-    <col min="21" max="21" hidden="false" style="1" width="27.9296296296296" collapsed="true"/>
-    <col min="22" max="22" hidden="false" style="0" width="43.7037037037037" collapsed="true"/>
-    <col min="23" max="23" hidden="false" style="0" width="32.337037037037" collapsed="true"/>
-    <col min="24" max="24" hidden="false" style="1" width="8.23333333333333" collapsed="true"/>
-    <col min="25" max="25" hidden="false" style="1" width="7.64444444444445" collapsed="true"/>
-    <col min="26" max="26" hidden="false" style="1" width="8.23333333333333" collapsed="true"/>
-    <col min="27" max="27" hidden="false" style="1" width="7.64444444444445" collapsed="true"/>
-    <col min="28" max="28" hidden="false" style="1" width="8.23333333333333" collapsed="true"/>
-    <col min="29" max="1025" hidden="false" style="0" width="8.81851851851852" collapsed="true"/>
+    <col min="16" max="16" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
+    <col min="17" max="17" hidden="false" style="1" width="6.17407407407407" collapsed="true"/>
+    <col min="18" max="18" hidden="false" style="1" width="5.78148148148148" collapsed="true"/>
+    <col min="19" max="19" hidden="false" style="1" width="10.1925925925926" collapsed="true"/>
+    <col min="20" max="20" hidden="false" style="1" width="16.2666666666667" collapsed="true"/>
+    <col min="21" max="21" hidden="false" style="1" width="26.7518518518519" collapsed="true"/>
+    <col min="22" max="22" hidden="false" style="0" width="41.6481481481481" collapsed="true"/>
+    <col min="23" max="23" hidden="false" style="0" width="30.7703703703704" collapsed="true"/>
+    <col min="24" max="24" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
+    <col min="25" max="25" hidden="false" style="1" width="7.44814814814815" collapsed="true"/>
+    <col min="26" max="26" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
+    <col min="27" max="27" hidden="false" style="1" width="7.44814814814815" collapsed="true"/>
+    <col min="28" max="28" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1" s="4">
@@ -1258,8 +1218,8 @@
       <c r="AB1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="5" t="s">
@@ -1310,6 +1270,8 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="5" t="s">
@@ -1370,6 +1332,8 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="5" t="s">
@@ -1430,6 +1394,8 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="5" t="s">
@@ -1484,6 +1450,8 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="5" t="s">
@@ -1546,44 +1514,46 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="5" t="s">
-        <v>310</v>
+        <v>53</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>311</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>312</v>
+        <v>55</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>313</v>
+        <v>56</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>314</v>
+        <v>57</v>
       </c>
       <c r="H7" s="6" t="n">
-        <v>1990.0</v>
+        <v>1990</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>315</v>
+        <v>58</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>316</v>
+        <v>38</v>
       </c>
       <c r="L7" s="6" t="n">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>317</v>
+        <v>39</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -1591,31 +1561,33 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="6" t="s">
-        <v>318</v>
+        <v>30</v>
       </c>
       <c r="T7" s="6" t="n">
-        <v>1996.0</v>
+        <v>1996</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>319</v>
+        <v>31</v>
       </c>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="6" t="s">
-        <v>320</v>
+        <v>59</v>
       </c>
       <c r="Y7" s="6" t="s">
-        <v>321</v>
+        <v>44</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>322</v>
+        <v>60</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>315</v>
+        <v>58</v>
       </c>
       <c r="AB7" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="5" t="s">
@@ -1668,6 +1640,8 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="5" t="s">
@@ -1720,6 +1694,8 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="5" t="s">
@@ -1780,6 +1756,8 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="5" t="s">
@@ -1832,6 +1810,8 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="5" t="s">
@@ -1892,6 +1872,8 @@
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="5" t="s">
@@ -1962,6 +1944,8 @@
       <c r="AB13" s="6" t="s">
         <v>84</v>
       </c>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="5" t="s">
@@ -2032,6 +2016,8 @@
       <c r="AB14" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="5" t="s">
@@ -2084,6 +2070,8 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="5" t="s">
@@ -2136,6 +2124,8 @@
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="5" t="s">
@@ -2186,6 +2176,8 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="5" t="s">
@@ -2256,6 +2248,8 @@
       <c r="AB18" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="5" t="s">
@@ -2312,6 +2306,8 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="5" t="s">
@@ -2382,6 +2378,8 @@
       <c r="AB20" s="6" t="s">
         <v>84</v>
       </c>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="5" t="s">
@@ -2432,6 +2430,8 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
       <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="5" t="s">
@@ -2484,6 +2484,8 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="5" t="s">
@@ -2554,6 +2556,8 @@
       <c r="AB23" s="6" t="s">
         <v>103</v>
       </c>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="5" t="s">
@@ -2616,6 +2620,8 @@
       <c r="AB24" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="5" t="s">
@@ -2692,6 +2698,8 @@
       <c r="AB25" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="5" t="s">
@@ -2750,6 +2758,8 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="5" t="s">
@@ -2802,6 +2812,8 @@
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
       <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="5" t="s">
@@ -2864,6 +2876,8 @@
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="A29" s="5" t="s">
@@ -2934,6 +2948,8 @@
       <c r="AB29" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="5" t="s">
@@ -2994,6 +3010,8 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
       <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="A31" s="5" t="s">
@@ -3056,6 +3074,8 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="5"/>
       <c r="AB31" s="5"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="A32" s="5" t="s">
@@ -3126,6 +3146,8 @@
       <c r="AB32" s="6" t="s">
         <v>103</v>
       </c>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="5" t="s">
@@ -3176,6 +3198,8 @@
       <c r="Z33" s="5"/>
       <c r="AA33" s="5"/>
       <c r="AB33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="5" t="s">
@@ -3246,6 +3270,8 @@
       <c r="AB34" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="AC34" s="5"/>
+      <c r="AD34" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="5" t="s">
@@ -3316,6 +3342,8 @@
       <c r="AB35" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="AC35" s="5"/>
+      <c r="AD35" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="5" t="s">
@@ -3386,6 +3414,8 @@
       <c r="AB36" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="AC36" s="5"/>
+      <c r="AD36" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="5" t="s">
@@ -3452,6 +3482,8 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
       <c r="AB37" s="5"/>
+      <c r="AC37" s="5"/>
+      <c r="AD37" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="5" t="s">
@@ -3522,6 +3554,8 @@
       <c r="AB38" s="6" t="s">
         <v>88</v>
       </c>
+      <c r="AC38" s="5"/>
+      <c r="AD38" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="5" t="s">
@@ -3582,6 +3616,8 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
       <c r="AB39" s="5"/>
+      <c r="AC39" s="5"/>
+      <c r="AD39" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="5" t="s">
@@ -3632,6 +3668,8 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
       <c r="AB40" s="5"/>
+      <c r="AC40" s="5"/>
+      <c r="AD40" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="5" t="s">
@@ -3692,6 +3730,8 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="5"/>
       <c r="AB41" s="5"/>
+      <c r="AC41" s="5"/>
+      <c r="AD41" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="5" t="s">
@@ -3762,6 +3802,8 @@
       <c r="AB42" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="AC42" s="5"/>
+      <c r="AD42" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="5" t="s">
@@ -3822,6 +3864,8 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
       <c r="AB43" s="5"/>
+      <c r="AC43" s="5"/>
+      <c r="AD43" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="5" t="s">
@@ -3882,6 +3926,8 @@
       <c r="AB44" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="AC44" s="5"/>
+      <c r="AD44" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="5" t="s">
@@ -3952,6 +3998,8 @@
       <c r="AB45" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="AC45" s="5"/>
+      <c r="AD45" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="5" t="s">
@@ -4008,6 +4056,8 @@
       </c>
       <c r="AA46" s="5"/>
       <c r="AB46" s="5"/>
+      <c r="AC46" s="5"/>
+      <c r="AD46" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="5" t="s">
@@ -4058,6 +4108,8 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
       <c r="AB47" s="5"/>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="48">
       <c r="A48" s="5" t="s">
@@ -4118,6 +4170,8 @@
       <c r="AB48" s="6" t="s">
         <v>84</v>
       </c>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="49">
       <c r="A49" s="5" t="s">
@@ -4178,6 +4232,8 @@
       <c r="Z49" s="5"/>
       <c r="AA49" s="5"/>
       <c r="AB49" s="5"/>
+      <c r="AC49" s="5"/>
+      <c r="AD49" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="A50" s="5" t="s">
@@ -4248,6 +4304,8 @@
       <c r="AB50" s="6" t="s">
         <v>58</v>
       </c>
+      <c r="AC50" s="5"/>
+      <c r="AD50" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="51">
       <c r="A51" s="5" t="s">
@@ -4318,6 +4376,8 @@
       <c r="AB51" s="6" t="s">
         <v>81</v>
       </c>
+      <c r="AC51" s="5"/>
+      <c r="AD51" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="52">
       <c r="A52" s="5" t="s">
@@ -4384,6 +4444,8 @@
       <c r="Z52" s="5"/>
       <c r="AA52" s="5"/>
       <c r="AB52" s="5"/>
+      <c r="AC52" s="5"/>
+      <c r="AD52" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="A53" s="5" t="s">
@@ -4444,6 +4506,8 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
       <c r="AB53" s="5"/>
+      <c r="AC53" s="5"/>
+      <c r="AD53" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="54">
       <c r="A54" s="5" t="s">
@@ -4514,6 +4578,8 @@
       <c r="AB54" s="6" t="s">
         <v>58</v>
       </c>
+      <c r="AC54" s="5"/>
+      <c r="AD54" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="55">
       <c r="A55" s="5" t="s">
@@ -4574,6 +4640,8 @@
       <c r="Z55" s="5"/>
       <c r="AA55" s="5"/>
       <c r="AB55" s="5"/>
+      <c r="AC55" s="5"/>
+      <c r="AD55" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="56">
       <c r="A56" s="5" t="s">
@@ -4624,6 +4692,8 @@
       <c r="Z56" s="5"/>
       <c r="AA56" s="5"/>
       <c r="AB56" s="5"/>
+      <c r="AC56" s="5"/>
+      <c r="AD56" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="57">
       <c r="A57" s="5" t="s">
@@ -4694,6 +4764,8 @@
       <c r="AB57" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="AC57" s="5"/>
+      <c r="AD57" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="58">
       <c r="A58" s="5" t="s">
@@ -4744,6 +4816,8 @@
       <c r="Z58" s="5"/>
       <c r="AA58" s="5"/>
       <c r="AB58" s="5"/>
+      <c r="AC58" s="5"/>
+      <c r="AD58" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="59">
       <c r="A59" s="5" t="s">
@@ -4814,6 +4888,8 @@
       <c r="AB59" s="6" t="s">
         <v>58</v>
       </c>
+      <c r="AC59" s="5"/>
+      <c r="AD59" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="60">
       <c r="A60" s="5" t="s">
@@ -4872,6 +4948,8 @@
       <c r="Z60" s="5"/>
       <c r="AA60" s="5"/>
       <c r="AB60" s="5"/>
+      <c r="AC60" s="5"/>
+      <c r="AD60" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="61">
       <c r="A61" s="5" t="s">
@@ -4942,6 +5020,8 @@
       <c r="AB61" s="6" t="s">
         <v>88</v>
       </c>
+      <c r="AC61" s="5"/>
+      <c r="AD61" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="62">
       <c r="A62" s="5" t="s">
@@ -5002,6 +5082,8 @@
       <c r="Z62" s="5"/>
       <c r="AA62" s="5"/>
       <c r="AB62" s="5"/>
+      <c r="AC62" s="5"/>
+      <c r="AD62" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="63">
       <c r="A63" s="5" t="s">
@@ -5072,6 +5154,8 @@
       <c r="AB63" s="6" t="s">
         <v>60</v>
       </c>
+      <c r="AC63" s="5"/>
+      <c r="AD63" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="64">
       <c r="A64" s="5" t="s">
@@ -5122,6 +5206,8 @@
       <c r="Z64" s="5"/>
       <c r="AA64" s="5"/>
       <c r="AB64" s="5"/>
+      <c r="AC64" s="5"/>
+      <c r="AD64" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="65">
       <c r="A65" s="5" t="s">
@@ -5192,6 +5278,8 @@
       <c r="AB65" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="AC65" s="5"/>
+      <c r="AD65" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="66">
       <c r="A66" s="5" t="s">
@@ -5262,6 +5350,8 @@
       <c r="AB66" s="6" t="s">
         <v>103</v>
       </c>
+      <c r="AC66" s="5"/>
+      <c r="AD66" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="67">
       <c r="A67" s="5" t="s">
@@ -5322,6 +5412,8 @@
       <c r="Z67" s="5"/>
       <c r="AA67" s="5"/>
       <c r="AB67" s="5"/>
+      <c r="AC67" s="5"/>
+      <c r="AD67" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="68">
       <c r="A68" s="5" t="s">
@@ -5392,6 +5484,8 @@
       <c r="AB68" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="AC68" s="5"/>
+      <c r="AD68" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="69">
       <c r="A69" s="5" t="s">
@@ -5442,6 +5536,8 @@
       <c r="Z69" s="5"/>
       <c r="AA69" s="5"/>
       <c r="AB69" s="5"/>
+      <c r="AC69" s="5"/>
+      <c r="AD69" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="70">
       <c r="A70" s="5" t="s">
@@ -5492,6 +5588,8 @@
       <c r="Z70" s="5"/>
       <c r="AA70" s="5"/>
       <c r="AB70" s="5"/>
+      <c r="AC70" s="5"/>
+      <c r="AD70" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="A71" s="5" t="s">
@@ -5568,6 +5666,8 @@
       <c r="AB71" s="6" t="s">
         <v>60</v>
       </c>
+      <c r="AC71" s="5"/>
+      <c r="AD71" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="72">
       <c r="A72" s="5" t="s">
@@ -5620,6 +5720,8 @@
       <c r="Z72" s="5"/>
       <c r="AA72" s="5"/>
       <c r="AB72" s="5"/>
+      <c r="AC72" s="5"/>
+      <c r="AD72" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="73">
       <c r="A73" s="5" t="s">
@@ -5690,6 +5792,8 @@
       <c r="AB73" s="6" t="s">
         <v>103</v>
       </c>
+      <c r="AC73" s="5"/>
+      <c r="AD73" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="74">
       <c r="A74" s="5" t="s">
@@ -5760,6 +5864,8 @@
       <c r="AB74" s="6" t="s">
         <v>103</v>
       </c>
+      <c r="AC74" s="5"/>
+      <c r="AD74" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="75">
       <c r="A75" s="5" t="s">
@@ -5830,6 +5936,8 @@
       <c r="AB75" s="6" t="s">
         <v>88</v>
       </c>
+      <c r="AC75" s="5"/>
+      <c r="AD75" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="76">
       <c r="A76" s="5" t="s">
@@ -5880,6 +5988,8 @@
       <c r="Z76" s="5"/>
       <c r="AA76" s="5"/>
       <c r="AB76" s="5"/>
+      <c r="AC76" s="5"/>
+      <c r="AD76" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="77">
       <c r="A77" s="5" t="s">
@@ -5930,6 +6040,8 @@
       <c r="Z77" s="5"/>
       <c r="AA77" s="5"/>
       <c r="AB77" s="5"/>
+      <c r="AC77" s="5"/>
+      <c r="AD77" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="78">
       <c r="A78" s="5" t="s">
@@ -5980,6 +6092,8 @@
       <c r="Z78" s="5"/>
       <c r="AA78" s="5"/>
       <c r="AB78" s="5"/>
+      <c r="AC78" s="5"/>
+      <c r="AD78" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="79">
       <c r="A79" s="5" t="s">
@@ -6030,6 +6144,8 @@
       <c r="Z79" s="5"/>
       <c r="AA79" s="5"/>
       <c r="AB79" s="5"/>
+      <c r="AC79" s="5"/>
+      <c r="AD79" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="80">
       <c r="A80" s="5" t="s">
@@ -6090,6 +6206,8 @@
       <c r="AB80" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="AC80" s="5"/>
+      <c r="AD80" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="81">
       <c r="A81" s="5" t="s">
@@ -6160,6 +6278,8 @@
       <c r="AB81" s="6" t="s">
         <v>58</v>
       </c>
+      <c r="AC81" s="5"/>
+      <c r="AD81" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="82">
       <c r="A82" s="5" t="s">
@@ -6210,6 +6330,8 @@
       <c r="Z82" s="5"/>
       <c r="AA82" s="5"/>
       <c r="AB82" s="5"/>
+      <c r="AC82" s="5"/>
+      <c r="AD82" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="83">
       <c r="A83" s="5" t="s">
@@ -6270,6 +6392,8 @@
       <c r="AB83" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="AC83" s="5"/>
+      <c r="AD83" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="84">
       <c r="A84" s="5" t="s">
@@ -6320,6 +6444,8 @@
       <c r="Z84" s="5"/>
       <c r="AA84" s="5"/>
       <c r="AB84" s="5"/>
+      <c r="AC84" s="5"/>
+      <c r="AD84" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="85">
       <c r="A85" s="5" t="s">
@@ -6380,6 +6506,8 @@
       <c r="Z85" s="5"/>
       <c r="AA85" s="5"/>
       <c r="AB85" s="5"/>
+      <c r="AC85" s="5"/>
+      <c r="AD85" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="86">
       <c r="A86" s="5" t="s">
@@ -6450,6 +6578,8 @@
       <c r="AB86" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="AC86" s="5"/>
+      <c r="AD86" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="87">
       <c r="A87" s="5" t="s">
@@ -6520,6 +6650,8 @@
       <c r="AB87" s="6" t="s">
         <v>88</v>
       </c>
+      <c r="AC87" s="5"/>
+      <c r="AD87" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="88">
       <c r="A88" s="5" t="s">
@@ -6580,6 +6712,8 @@
       <c r="AB88" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="AC88" s="5"/>
+      <c r="AD88" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="89">
       <c r="A89" s="5" t="s">
@@ -6640,6 +6774,8 @@
       <c r="AB89" s="6" t="s">
         <v>84</v>
       </c>
+      <c r="AC89" s="5"/>
+      <c r="AD89" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="90">
       <c r="A90" s="5" t="s">
@@ -6690,6 +6826,8 @@
       <c r="Z90" s="5"/>
       <c r="AA90" s="5"/>
       <c r="AB90" s="5"/>
+      <c r="AC90" s="5"/>
+      <c r="AD90" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="91">
       <c r="A91" s="5" t="s">
@@ -6740,6 +6878,8 @@
       <c r="Z91" s="5"/>
       <c r="AA91" s="5"/>
       <c r="AB91" s="5"/>
+      <c r="AC91" s="5"/>
+      <c r="AD91" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="92">
       <c r="A92" s="5" t="s">
@@ -6800,6 +6940,8 @@
       <c r="AB92" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="AC92" s="5"/>
+      <c r="AD92" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="93">
       <c r="A93" s="5" t="s">
@@ -6850,6 +6992,8 @@
       <c r="Z93" s="5"/>
       <c r="AA93" s="5"/>
       <c r="AB93" s="5"/>
+      <c r="AC93" s="5"/>
+      <c r="AD93" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="94">
       <c r="A94" s="5" t="s">
@@ -6910,6 +7054,8 @@
       <c r="AB94" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="AC94" s="5"/>
+      <c r="AD94" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="95">
       <c r="A95" s="5" t="s">
@@ -6960,6 +7106,8 @@
       <c r="Z95" s="5"/>
       <c r="AA95" s="5"/>
       <c r="AB95" s="5"/>
+      <c r="AC95" s="5"/>
+      <c r="AD95" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="96">
       <c r="A96" s="5" t="s">
@@ -7020,6 +7168,8 @@
       <c r="AB96" s="6" t="s">
         <v>81</v>
       </c>
+      <c r="AC96" s="5"/>
+      <c r="AD96" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="97">
       <c r="A97" s="5" t="s">
@@ -7080,6 +7230,8 @@
       <c r="AB97" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="AC97" s="5"/>
+      <c r="AD97" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="98">
       <c r="A98" s="5" t="s">
@@ -7130,6 +7282,8 @@
       <c r="Z98" s="6"/>
       <c r="AA98" s="6"/>
       <c r="AB98" s="6"/>
+      <c r="AC98" s="5"/>
+      <c r="AD98" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="99">
       <c r="A99" s="5" t="s">
@@ -7180,6 +7334,8 @@
       <c r="Z99" s="6"/>
       <c r="AA99" s="6"/>
       <c r="AB99" s="6"/>
+      <c r="AC99" s="5"/>
+      <c r="AD99" s="5"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
@@ -7205,8 +7361,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="88.7814814814815" collapsed="true"/>
-    <col min="2" max="1025" hidden="false" style="0" width="9.40740740740741" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="84.4703703703704" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="9.01481481481481" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Got save working! Also got the edit professor working.
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="325">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -182,10 +182,10 @@
     <t xml:space="preserve">L</t>
   </si>
   <si>
-    <t xml:space="preserve">Geoff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pullum</t>
+    <t xml:space="preserve">please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work</t>
   </si>
   <si>
     <t xml:space="preserve">HSS</t>
@@ -951,6 +951,51 @@
   </si>
   <si>
     <t xml:space="preserve">FacChair is not elegible for election or appointment to a committee</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>better work</t>
+  </si>
+  <si>
+    <t>5654</t>
+  </si>
+  <si>
+    <t>HSS</t>
+  </si>
+  <si>
+    <t>Lang &amp; Literature</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>AASFA</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>VALC</t>
+  </si>
+  <si>
+    <t>FERC</t>
+  </si>
+  <si>
+    <t>Lib</t>
   </si>
 </sst>
 </file>
@@ -1097,40 +1142,41 @@
   </sheetPr>
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A49" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
       <selection activeCell="M88" activeCellId="0" pane="topLeft" sqref="M88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="12.837037037037" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="15.3851851851852" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="13.1296296296296" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="15.7777777777778" collapsed="true"/>
     <col min="3" max="3" hidden="false" style="1" width="3.33333333333333" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="1" width="13.1296296296296" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="1" width="9.9962962962963" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="17.2481481481481" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="18.5222222222222" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="1" width="22.8333333333333" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="1" width="13.4259259259259" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="1" width="10.1925925925926" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="17.6407407407407" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="18.9111111111111" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="1" width="16.0703703703704" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="1" width="23.3222222222222" collapsed="true"/>
     <col min="10" max="10" hidden="false" style="1" width="3.23333333333333" collapsed="true"/>
-    <col min="11" max="11" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
-    <col min="12" max="12" hidden="false" style="1" width="6.17407407407407" collapsed="true"/>
-    <col min="13" max="13" hidden="false" style="1" width="5.78148148148148" collapsed="true"/>
-    <col min="14" max="14" hidden="false" style="1" width="19.7962962962963" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="1" width="16.0703703703704" collapsed="true"/>
+    <col min="12" max="12" hidden="false" style="1" width="6.27037037037037" collapsed="true"/>
+    <col min="13" max="13" hidden="false" style="1" width="5.88148148148148" collapsed="true"/>
+    <col min="14" max="14" hidden="false" style="1" width="20.2851851851852" collapsed="true"/>
     <col min="15" max="15" hidden="false" style="1" width="2.35185185185185" collapsed="true"/>
-    <col min="16" max="16" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
-    <col min="17" max="17" hidden="false" style="1" width="6.17407407407407" collapsed="true"/>
-    <col min="18" max="18" hidden="false" style="1" width="5.78148148148148" collapsed="true"/>
-    <col min="19" max="19" hidden="false" style="1" width="10.1925925925926" collapsed="true"/>
-    <col min="20" max="20" hidden="false" style="1" width="16.2666666666667" collapsed="true"/>
-    <col min="21" max="21" hidden="false" style="1" width="26.7518518518519" collapsed="true"/>
-    <col min="22" max="22" hidden="false" style="0" width="41.6481481481481" collapsed="true"/>
-    <col min="23" max="23" hidden="false" style="0" width="30.7703703703704" collapsed="true"/>
-    <col min="24" max="24" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
-    <col min="25" max="25" hidden="false" style="1" width="7.44814814814815" collapsed="true"/>
-    <col min="26" max="26" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
-    <col min="27" max="27" hidden="false" style="1" width="7.44814814814815" collapsed="true"/>
-    <col min="28" max="28" hidden="false" style="1" width="8.03703703703704" collapsed="true"/>
+    <col min="16" max="16" hidden="false" style="1" width="16.0703703703704" collapsed="true"/>
+    <col min="17" max="17" hidden="false" style="1" width="6.27037037037037" collapsed="true"/>
+    <col min="18" max="18" hidden="false" style="1" width="5.88148148148148" collapsed="true"/>
+    <col min="19" max="19" hidden="false" style="1" width="10.3888888888889" collapsed="true"/>
+    <col min="20" max="20" hidden="false" style="1" width="16.6592592592593" collapsed="true"/>
+    <col min="21" max="21" hidden="false" style="1" width="27.3407407407407" collapsed="true"/>
+    <col min="22" max="22" hidden="false" style="0" width="42.6259259259259" collapsed="true"/>
+    <col min="23" max="23" hidden="false" style="0" width="31.5555555555556" collapsed="true"/>
+    <col min="24" max="24" hidden="false" style="1" width="8.13333333333333" collapsed="true"/>
+    <col min="25" max="25" hidden="false" style="1" width="7.54444444444444" collapsed="true"/>
+    <col min="26" max="26" hidden="false" style="1" width="8.13333333333333" collapsed="true"/>
+    <col min="27" max="27" hidden="false" style="1" width="7.54444444444444" collapsed="true"/>
+    <col min="28" max="28" hidden="false" style="1" width="8.13333333333333" collapsed="true"/>
+    <col min="29" max="1025" hidden="false" style="0" width="8.62222222222222" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1" s="4">
@@ -1519,69 +1565,85 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="5" t="s">
-        <v>53</v>
+        <v>310</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>54</v>
+        <v>311</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>6.0</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>312</v>
+      </c>
       <c r="E7" s="6" t="s">
-        <v>55</v>
+        <v>313</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>56</v>
+        <v>314</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>57</v>
+        <v>315</v>
       </c>
       <c r="H7" s="6" t="n">
-        <v>1990</v>
+        <v>1990.0</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>58</v>
+        <v>316</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>38</v>
+        <v>317</v>
       </c>
       <c r="L7" s="6" t="n">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
+        <v>318</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="S7" s="6" t="s">
-        <v>30</v>
+        <v>320</v>
       </c>
       <c r="T7" s="6" t="n">
-        <v>1996</v>
+        <v>1996.0</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
+        <v>321</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="X7" s="6" t="s">
-        <v>59</v>
+        <v>322</v>
       </c>
       <c r="Y7" s="6" t="s">
-        <v>44</v>
+        <v>323</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>60</v>
+        <v>324</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>58</v>
+        <v>316</v>
       </c>
       <c r="AB7" s="6" t="s">
         <v>61</v>
@@ -7361,8 +7423,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="84.4703703703704" collapsed="true"/>
-    <col min="2" max="1025" hidden="false" style="0" width="9.01481481481481" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="86.6259259259259" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="9.21111111111111" collapsed="true"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Standard Requirements are complete. Next I need to start working on the requirements for each committee.
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -2,16 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" date1904="true" showObjects="all"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="992" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="CoC with simplified tenure trac" r:id="rId2" sheetId="1" state="visible"/>
-    <sheet name="CoC Specs" r:id="rId3" sheetId="2" state="visible"/>
+    <sheet name="CoC with simplified tenure trac" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="CoC Specs" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterate="false" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="310">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -182,10 +182,10 @@
     <t xml:space="preserve">L</t>
   </si>
   <si>
-    <t xml:space="preserve">please</t>
-  </si>
-  <si>
-    <t xml:space="preserve">work</t>
+    <t xml:space="preserve">Geoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pullum</t>
   </si>
   <si>
     <t xml:space="preserve">HSS</t>
@@ -951,51 +951,6 @@
   </si>
   <si>
     <t xml:space="preserve">FacChair is not elegible for election or appointment to a committee</t>
-  </si>
-  <si>
-    <t>this</t>
-  </si>
-  <si>
-    <t>better work</t>
-  </si>
-  <si>
-    <t>5654</t>
-  </si>
-  <si>
-    <t>HSS</t>
-  </si>
-  <si>
-    <t>Lang &amp; Literature</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>AASFA</t>
-  </si>
-  <si>
-    <t>DIV</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Professor</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>VALC</t>
-  </si>
-  <si>
-    <t>FERC</t>
-  </si>
-  <si>
-    <t>Lib</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1016,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -1070,67 +1025,67 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -1142,44 +1097,44 @@
   </sheetPr>
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="M88" activeCellId="0" pane="topLeft" sqref="M88"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="13.1296296296296" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="15.7777777777778" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="1" width="3.33333333333333" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="1" width="13.4259259259259" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="1" width="10.1925925925926" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="17.6407407407407" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="18.9111111111111" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="1" width="16.0703703703704" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="1" width="23.3222222222222" collapsed="true"/>
-    <col min="10" max="10" hidden="false" style="1" width="3.23333333333333" collapsed="true"/>
-    <col min="11" max="11" hidden="false" style="1" width="16.0703703703704" collapsed="true"/>
-    <col min="12" max="12" hidden="false" style="1" width="6.27037037037037" collapsed="true"/>
-    <col min="13" max="13" hidden="false" style="1" width="5.88148148148148" collapsed="true"/>
-    <col min="14" max="14" hidden="false" style="1" width="20.2851851851852" collapsed="true"/>
-    <col min="15" max="15" hidden="false" style="1" width="2.35185185185185" collapsed="true"/>
-    <col min="16" max="16" hidden="false" style="1" width="16.0703703703704" collapsed="true"/>
-    <col min="17" max="17" hidden="false" style="1" width="6.27037037037037" collapsed="true"/>
-    <col min="18" max="18" hidden="false" style="1" width="5.88148148148148" collapsed="true"/>
-    <col min="19" max="19" hidden="false" style="1" width="10.3888888888889" collapsed="true"/>
-    <col min="20" max="20" hidden="false" style="1" width="16.6592592592593" collapsed="true"/>
-    <col min="21" max="21" hidden="false" style="1" width="27.3407407407407" collapsed="true"/>
-    <col min="22" max="22" hidden="false" style="0" width="42.6259259259259" collapsed="true"/>
-    <col min="23" max="23" hidden="false" style="0" width="31.5555555555556" collapsed="true"/>
-    <col min="24" max="24" hidden="false" style="1" width="8.13333333333333" collapsed="true"/>
-    <col min="25" max="25" hidden="false" style="1" width="7.54444444444444" collapsed="true"/>
-    <col min="26" max="26" hidden="false" style="1" width="8.13333333333333" collapsed="true"/>
-    <col min="27" max="27" hidden="false" style="1" width="7.54444444444444" collapsed="true"/>
-    <col min="28" max="28" hidden="false" style="1" width="8.13333333333333" collapsed="true"/>
-    <col min="29" max="1025" hidden="false" style="0" width="8.62222222222222" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="3.33333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="3.23333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="6.27037037037037"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="2.35185185185185"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="6.27037037037037"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="42.6259259259259"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="8.13333333333333"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="7.54444444444444"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="8.13333333333333"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.54444444444444"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="8.13333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1" s="4">
+    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1222,7 @@
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -1319,7 +1274,7 @@
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -1352,7 +1307,7 @@
         <v>38</v>
       </c>
       <c r="L3" s="6" t="n">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>39</v>
@@ -1381,7 +1336,7 @@
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>40</v>
       </c>
@@ -1443,7 +1398,7 @@
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>45</v>
       </c>
@@ -1499,7 +1454,7 @@
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -1563,87 +1518,71 @@
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>310</v>
+        <v>53</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>311</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>312</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>313</v>
+        <v>55</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>314</v>
+        <v>56</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>315</v>
+        <v>57</v>
       </c>
       <c r="H7" s="6" t="n">
-        <v>1990.0</v>
+        <v>1990</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>316</v>
+        <v>58</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>317</v>
+        <v>38</v>
       </c>
       <c r="L7" s="6" t="n">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>319</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
       <c r="S7" s="6" t="s">
-        <v>320</v>
+        <v>30</v>
       </c>
       <c r="T7" s="6" t="n">
-        <v>1996.0</v>
+        <v>1996</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="V7" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>319</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
       <c r="X7" s="6" t="s">
-        <v>322</v>
+        <v>59</v>
       </c>
       <c r="Y7" s="6" t="s">
-        <v>323</v>
+        <v>44</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>324</v>
+        <v>60</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>316</v>
+        <v>58</v>
       </c>
       <c r="AB7" s="6" t="s">
         <v>61</v>
@@ -1651,7 +1590,7 @@
       <c r="AC7" s="5"/>
       <c r="AD7" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>62</v>
       </c>
@@ -1705,7 +1644,7 @@
       <c r="AC8" s="5"/>
       <c r="AD8" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>66</v>
       </c>
@@ -1759,7 +1698,7 @@
       <c r="AC9" s="5"/>
       <c r="AD9" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>70</v>
       </c>
@@ -1821,7 +1760,7 @@
       <c r="AC10" s="5"/>
       <c r="AD10" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>74</v>
       </c>
@@ -1875,7 +1814,7 @@
       <c r="AC11" s="5"/>
       <c r="AD11" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>79</v>
       </c>
@@ -1937,7 +1876,7 @@
       <c r="AC12" s="5"/>
       <c r="AD12" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>82</v>
       </c>
@@ -2009,7 +1948,7 @@
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
@@ -2081,7 +2020,7 @@
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
         <v>89</v>
       </c>
@@ -2135,7 +2074,7 @@
       <c r="AC15" s="5"/>
       <c r="AD15" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>94</v>
       </c>
@@ -2189,7 +2128,7 @@
       <c r="AC16" s="5"/>
       <c r="AD16" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>97</v>
       </c>
@@ -2241,7 +2180,7 @@
       <c r="AC17" s="5"/>
       <c r="AD17" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
         <v>99</v>
       </c>
@@ -2313,7 +2252,7 @@
       <c r="AC18" s="5"/>
       <c r="AD18" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>104</v>
       </c>
@@ -2371,7 +2310,7 @@
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
         <v>107</v>
       </c>
@@ -2443,7 +2382,7 @@
       <c r="AC20" s="5"/>
       <c r="AD20" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
         <v>109</v>
       </c>
@@ -2495,7 +2434,7 @@
       <c r="AC21" s="5"/>
       <c r="AD21" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>116</v>
       </c>
@@ -2549,7 +2488,7 @@
       <c r="AC22" s="5"/>
       <c r="AD22" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>118</v>
       </c>
@@ -2621,7 +2560,7 @@
       <c r="AC23" s="5"/>
       <c r="AD23" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
@@ -2685,7 +2624,7 @@
       <c r="AC24" s="5"/>
       <c r="AD24" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>125</v>
       </c>
@@ -2763,7 +2702,7 @@
       <c r="AC25" s="5"/>
       <c r="AD25" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
         <v>107</v>
       </c>
@@ -2823,7 +2762,7 @@
       <c r="AC26" s="5"/>
       <c r="AD26" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>131</v>
       </c>
@@ -2877,7 +2816,7 @@
       <c r="AC27" s="5"/>
       <c r="AD27" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>134</v>
       </c>
@@ -2941,7 +2880,7 @@
       <c r="AC28" s="5"/>
       <c r="AD28" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
         <v>136</v>
       </c>
@@ -3013,7 +2952,7 @@
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
         <v>138</v>
       </c>
@@ -3075,7 +3014,7 @@
       <c r="AC30" s="5"/>
       <c r="AD30" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
         <v>140</v>
       </c>
@@ -3139,7 +3078,7 @@
       <c r="AC31" s="5"/>
       <c r="AD31" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
         <v>143</v>
       </c>
@@ -3211,7 +3150,7 @@
       <c r="AC32" s="5"/>
       <c r="AD32" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
         <v>145</v>
       </c>
@@ -3263,7 +3202,7 @@
       <c r="AC33" s="5"/>
       <c r="AD33" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
         <v>149</v>
       </c>
@@ -3335,7 +3274,7 @@
       <c r="AC34" s="5"/>
       <c r="AD34" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
         <v>151</v>
       </c>
@@ -3407,7 +3346,7 @@
       <c r="AC35" s="5"/>
       <c r="AD35" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
         <v>153</v>
       </c>
@@ -3479,7 +3418,7 @@
       <c r="AC36" s="5"/>
       <c r="AD36" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
         <v>155</v>
       </c>
@@ -3547,7 +3486,7 @@
       <c r="AC37" s="5"/>
       <c r="AD37" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="38">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
         <v>157</v>
       </c>
@@ -3619,7 +3558,7 @@
       <c r="AC38" s="5"/>
       <c r="AD38" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="39">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
         <v>159</v>
       </c>
@@ -3681,7 +3620,7 @@
       <c r="AC39" s="5"/>
       <c r="AD39" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="40">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
         <v>161</v>
       </c>
@@ -3733,7 +3672,7 @@
       <c r="AC40" s="5"/>
       <c r="AD40" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="41">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
         <v>163</v>
       </c>
@@ -3795,7 +3734,7 @@
       <c r="AC41" s="5"/>
       <c r="AD41" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="42">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
         <v>166</v>
       </c>
@@ -3867,7 +3806,7 @@
       <c r="AC42" s="5"/>
       <c r="AD42" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="43">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
         <v>168</v>
       </c>
@@ -3929,7 +3868,7 @@
       <c r="AC43" s="5"/>
       <c r="AD43" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="44">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
         <v>170</v>
       </c>
@@ -3991,7 +3930,7 @@
       <c r="AC44" s="5"/>
       <c r="AD44" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="45">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
         <v>172</v>
       </c>
@@ -4063,7 +4002,7 @@
       <c r="AC45" s="5"/>
       <c r="AD45" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="46">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
         <v>174</v>
       </c>
@@ -4121,7 +4060,7 @@
       <c r="AC46" s="5"/>
       <c r="AD46" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="47">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
         <v>176</v>
       </c>
@@ -4173,7 +4112,7 @@
       <c r="AC47" s="5"/>
       <c r="AD47" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="48">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
         <v>178</v>
       </c>
@@ -4235,7 +4174,7 @@
       <c r="AC48" s="5"/>
       <c r="AD48" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="49">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
         <v>180</v>
       </c>
@@ -4297,7 +4236,7 @@
       <c r="AC49" s="5"/>
       <c r="AD49" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="50">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
         <v>182</v>
       </c>
@@ -4369,7 +4308,7 @@
       <c r="AC50" s="5"/>
       <c r="AD50" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="51">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
         <v>184</v>
       </c>
@@ -4441,7 +4380,7 @@
       <c r="AC51" s="5"/>
       <c r="AD51" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="52">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
         <v>140</v>
       </c>
@@ -4509,7 +4448,7 @@
       <c r="AC52" s="5"/>
       <c r="AD52" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="53">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
         <v>188</v>
       </c>
@@ -4571,7 +4510,7 @@
       <c r="AC53" s="5"/>
       <c r="AD53" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="54">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
         <v>62</v>
       </c>
@@ -4643,7 +4582,7 @@
       <c r="AC54" s="5"/>
       <c r="AD54" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="55">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
         <v>191</v>
       </c>
@@ -4705,7 +4644,7 @@
       <c r="AC55" s="5"/>
       <c r="AD55" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="56">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
         <v>192</v>
       </c>
@@ -4757,7 +4696,7 @@
       <c r="AC56" s="5"/>
       <c r="AD56" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="57">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
         <v>195</v>
       </c>
@@ -4829,7 +4768,7 @@
       <c r="AC57" s="5"/>
       <c r="AD57" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="58">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
         <v>198</v>
       </c>
@@ -4881,7 +4820,7 @@
       <c r="AC58" s="5"/>
       <c r="AD58" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="59">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
         <v>138</v>
       </c>
@@ -4953,7 +4892,7 @@
       <c r="AC59" s="5"/>
       <c r="AD59" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="60">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
         <v>202</v>
       </c>
@@ -5013,7 +4952,7 @@
       <c r="AC60" s="5"/>
       <c r="AD60" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="61">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
         <v>205</v>
       </c>
@@ -5085,7 +5024,7 @@
       <c r="AC61" s="5"/>
       <c r="AD61" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="62">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
         <v>207</v>
       </c>
@@ -5147,7 +5086,7 @@
       <c r="AC62" s="5"/>
       <c r="AD62" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="63">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
         <v>209</v>
       </c>
@@ -5219,7 +5158,7 @@
       <c r="AC63" s="5"/>
       <c r="AD63" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="64">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
         <v>211</v>
       </c>
@@ -5271,7 +5210,7 @@
       <c r="AC64" s="5"/>
       <c r="AD64" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="65">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
         <v>213</v>
       </c>
@@ -5343,7 +5282,7 @@
       <c r="AC65" s="5"/>
       <c r="AD65" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="66">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
         <v>215</v>
       </c>
@@ -5415,7 +5354,7 @@
       <c r="AC66" s="5"/>
       <c r="AD66" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="67">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
         <v>217</v>
       </c>
@@ -5477,7 +5416,7 @@
       <c r="AC67" s="5"/>
       <c r="AD67" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="68">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
         <v>62</v>
       </c>
@@ -5549,7 +5488,7 @@
       <c r="AC68" s="5"/>
       <c r="AD68" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="69">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
         <v>221</v>
       </c>
@@ -5601,7 +5540,7 @@
       <c r="AC69" s="5"/>
       <c r="AD69" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="70">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
         <v>223</v>
       </c>
@@ -5653,7 +5592,7 @@
       <c r="AC70" s="5"/>
       <c r="AD70" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="71">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
         <v>225</v>
       </c>
@@ -5731,7 +5670,7 @@
       <c r="AC71" s="5"/>
       <c r="AD71" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="72">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
         <v>227</v>
       </c>
@@ -5785,7 +5724,7 @@
       <c r="AC72" s="5"/>
       <c r="AD72" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="73">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
         <v>47</v>
       </c>
@@ -5857,7 +5796,7 @@
       <c r="AC73" s="5"/>
       <c r="AD73" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="74">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
         <v>233</v>
       </c>
@@ -5929,7 +5868,7 @@
       <c r="AC74" s="5"/>
       <c r="AD74" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="75">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
         <v>178</v>
       </c>
@@ -6001,7 +5940,7 @@
       <c r="AC75" s="5"/>
       <c r="AD75" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="76">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>82</v>
       </c>
@@ -6053,7 +5992,7 @@
       <c r="AC76" s="5"/>
       <c r="AD76" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="77">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
         <v>237</v>
       </c>
@@ -6105,7 +6044,7 @@
       <c r="AC77" s="5"/>
       <c r="AD77" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="78">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="s">
         <v>239</v>
       </c>
@@ -6157,7 +6096,7 @@
       <c r="AC78" s="5"/>
       <c r="AD78" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="79">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
         <v>241</v>
       </c>
@@ -6209,7 +6148,7 @@
       <c r="AC79" s="5"/>
       <c r="AD79" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="80">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
         <v>62</v>
       </c>
@@ -6271,7 +6210,7 @@
       <c r="AC80" s="5"/>
       <c r="AD80" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="81">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
         <v>244</v>
       </c>
@@ -6343,7 +6282,7 @@
       <c r="AC81" s="5"/>
       <c r="AD81" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="82">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
         <v>245</v>
       </c>
@@ -6395,7 +6334,7 @@
       <c r="AC82" s="5"/>
       <c r="AD82" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="83">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
         <v>247</v>
       </c>
@@ -6457,7 +6396,7 @@
       <c r="AC83" s="5"/>
       <c r="AD83" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="84">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
         <v>249</v>
       </c>
@@ -6509,7 +6448,7 @@
       <c r="AC84" s="5"/>
       <c r="AD84" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="85">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="5" t="s">
         <v>168</v>
       </c>
@@ -6571,7 +6510,7 @@
       <c r="AC85" s="5"/>
       <c r="AD85" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="86">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
         <v>253</v>
       </c>
@@ -6643,7 +6582,7 @@
       <c r="AC86" s="5"/>
       <c r="AD86" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="87">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
         <v>256</v>
       </c>
@@ -6715,7 +6654,7 @@
       <c r="AC87" s="5"/>
       <c r="AD87" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="88">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
         <v>258</v>
       </c>
@@ -6777,7 +6716,7 @@
       <c r="AC88" s="5"/>
       <c r="AD88" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="89">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
         <v>260</v>
       </c>
@@ -6839,7 +6778,7 @@
       <c r="AC89" s="5"/>
       <c r="AD89" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="90">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
         <v>262</v>
       </c>
@@ -6891,7 +6830,7 @@
       <c r="AC90" s="5"/>
       <c r="AD90" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="91">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
         <v>205</v>
       </c>
@@ -6943,7 +6882,7 @@
       <c r="AC91" s="5"/>
       <c r="AD91" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="92">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
         <v>266</v>
       </c>
@@ -7005,7 +6944,7 @@
       <c r="AC92" s="5"/>
       <c r="AD92" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="93">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
         <v>268</v>
       </c>
@@ -7057,7 +6996,7 @@
       <c r="AC93" s="5"/>
       <c r="AD93" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="94">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
         <v>25</v>
       </c>
@@ -7119,7 +7058,7 @@
       <c r="AC94" s="5"/>
       <c r="AD94" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="95">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
         <v>271</v>
       </c>
@@ -7171,7 +7110,7 @@
       <c r="AC95" s="5"/>
       <c r="AD95" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="96">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
         <v>273</v>
       </c>
@@ -7233,7 +7172,7 @@
       <c r="AC96" s="5"/>
       <c r="AD96" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="97">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
         <v>275</v>
       </c>
@@ -7295,7 +7234,7 @@
       <c r="AC97" s="5"/>
       <c r="AD97" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="98">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
         <v>277</v>
       </c>
@@ -7347,7 +7286,7 @@
       <c r="AC98" s="5"/>
       <c r="AD98" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="99">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
         <v>178</v>
       </c>
@@ -7400,9 +7339,9 @@
       <c r="AD99" s="5"/>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7417,17 +7356,17 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="H9" activeCellId="0" pane="topLeft" sqref="H9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="86.6259259259259" collapsed="true"/>
-    <col min="2" max="1025" hidden="false" style="0" width="9.21111111111111" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="86.6259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>280</v>
       </c>
@@ -7449,7 +7388,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
         <v>284</v>
@@ -7471,7 +7410,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>288</v>
       </c>
@@ -7497,7 +7436,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -7511,7 +7450,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -7541,7 +7480,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
@@ -7571,7 +7510,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>290</v>
       </c>
@@ -7601,7 +7540,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -7631,7 +7570,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>293</v>
       </c>
@@ -7661,7 +7600,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>81</v>
       </c>
@@ -7691,7 +7630,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>296</v>
       </c>
@@ -7713,7 +7652,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>298</v>
       </c>
@@ -7735,7 +7674,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>299</v>
       </c>
@@ -7757,7 +7696,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>59</v>
       </c>
@@ -7787,7 +7726,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
         <v>300</v>
       </c>
@@ -7809,7 +7748,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -7823,7 +7762,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>301</v>
       </c>
@@ -7839,7 +7778,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
         <v>302</v>
       </c>
@@ -7855,7 +7794,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>303</v>
       </c>
@@ -7871,7 +7810,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
         <v>304</v>
       </c>
@@ -7887,7 +7826,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
         <v>305</v>
       </c>
@@ -7903,7 +7842,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>306</v>
       </c>
@@ -7919,7 +7858,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>307</v>
       </c>
@@ -7935,7 +7874,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>308</v>
       </c>
@@ -7951,7 +7890,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>309</v>
       </c>
@@ -7968,9 +7907,9 @@
       <c r="L25" s="5"/>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Fixed edit professor by checking if a cell is null, then create a cell in its spot
</commit_message>
<xml_diff>
--- a/Committee_on_Committes/CoC.xlsx
+++ b/Committee_on_Committes/CoC.xlsx
@@ -2,16 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
+  <workbookPr backupFile="false" date1904="true" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="990" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="CoC with simplified tenure trac" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CoC with simplified tenure trac" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="Sheet2" r:id="rId3" sheetId="2" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="321">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -942,6 +942,48 @@
   </si>
   <si>
     <t xml:space="preserve">FacChair is not elegible for election or appointment to a committee</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Pullum</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>HSS</t>
+  </si>
+  <si>
+    <t>Lang &amp; Literature</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>AASFA</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>VALC</t>
+  </si>
+  <si>
+    <t>FERC</t>
+  </si>
+  <si>
+    <t>Lib</t>
   </si>
 </sst>
 </file>
@@ -990,7 +1032,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -999,59 +1041,59 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -1063,44 +1105,44 @@
   </sheetPr>
   <dimension ref="A1:AB99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="3.23333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.93703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="3.23333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="5.29259259259259"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="4.9"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="3.23333333333333"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="5.29259259259259"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="4.9"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="32.8296296296296"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="6.85925925925926"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="6.85925925925926"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="10.6814814814815"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.9555555555556" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="14.1111111111111" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="1" width="3.23333333333333" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="1" width="10.6814814814815" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="1" width="7.93703703703704" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="15.6777777777778" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="17.0518518518519" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="1" width="12.4444444444444" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="1" width="18.1296296296296" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="1" width="3.23333333333333" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="1" width="12.4444444444444" collapsed="true"/>
+    <col min="12" max="12" hidden="false" style="1" width="5.29259259259259" collapsed="true"/>
+    <col min="13" max="13" hidden="false" style="1" width="4.9" collapsed="true"/>
+    <col min="14" max="14" hidden="false" style="1" width="15.6777777777778" collapsed="true"/>
+    <col min="15" max="15" hidden="false" style="1" width="3.23333333333333" collapsed="true"/>
+    <col min="16" max="16" hidden="false" style="1" width="12.4444444444444" collapsed="true"/>
+    <col min="17" max="17" hidden="false" style="1" width="5.29259259259259" collapsed="true"/>
+    <col min="18" max="18" hidden="false" style="1" width="4.9" collapsed="true"/>
+    <col min="19" max="19" hidden="false" style="1" width="9.40740740740741" collapsed="true"/>
+    <col min="20" max="20" hidden="false" style="1" width="13.1296296296296" collapsed="true"/>
+    <col min="21" max="21" hidden="false" style="1" width="21.1666666666667" collapsed="true"/>
+    <col min="22" max="22" hidden="false" style="0" width="32.8296296296296" collapsed="true"/>
+    <col min="23" max="23" hidden="false" style="0" width="24.3037037037037" collapsed="true"/>
+    <col min="24" max="24" hidden="false" style="1" width="7.64444444444445" collapsed="true"/>
+    <col min="25" max="25" hidden="false" style="1" width="6.85925925925926" collapsed="true"/>
+    <col min="26" max="26" hidden="false" style="1" width="7.64444444444445" collapsed="true"/>
+    <col min="27" max="27" hidden="false" style="1" width="6.85925925925926" collapsed="true"/>
+    <col min="28" max="28" hidden="false" style="1" width="7.64444444444445" collapsed="true"/>
+    <col min="29" max="1025" hidden="false" style="0" width="10.6814814814815" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1" s="2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +1228,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1234,7 +1276,7 @@
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -1292,7 +1334,7 @@
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="4" t="s">
         <v>40</v>
       </c>
@@ -1350,7 +1392,7 @@
       <c r="AA4" s="0"/>
       <c r="AB4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
@@ -1402,7 +1444,7 @@
       <c r="AA5" s="0"/>
       <c r="AB5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
@@ -1462,75 +1504,87 @@
       <c r="AA6" s="0"/>
       <c r="AB6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="4" t="s">
-        <v>53</v>
+        <v>307</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>54</v>
+        <v>308</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0"/>
+        <v>6.0</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>309</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>310</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>56</v>
+        <v>311</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>57</v>
+        <v>312</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>1990</v>
+        <v>1990.0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>58</v>
+        <v>313</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>38</v>
+        <v>314</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>2018</v>
+        <v>2018.0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="0"/>
-      <c r="O7" s="0"/>
-      <c r="P7" s="0"/>
-      <c r="Q7" s="0"/>
-      <c r="R7" s="0"/>
+        <v>315</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>309</v>
+      </c>
       <c r="S7" s="1" t="s">
-        <v>30</v>
+        <v>316</v>
       </c>
       <c r="T7" s="1" t="n">
-        <v>1996</v>
+        <v>1996.0</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>31</v>
+        <v>317</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>59</v>
+        <v>318</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>44</v>
+        <v>319</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>60</v>
+        <v>320</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>58</v>
+        <v>313</v>
       </c>
       <c r="AB7" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="4" t="s">
         <v>62</v>
       </c>
@@ -1580,7 +1634,7 @@
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
@@ -1630,7 +1684,7 @@
       <c r="AA9" s="0"/>
       <c r="AB9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="4" t="s">
         <v>70</v>
       </c>
@@ -1688,7 +1742,7 @@
       <c r="AA10" s="0"/>
       <c r="AB10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="4" t="s">
         <v>74</v>
       </c>
@@ -1738,7 +1792,7 @@
       <c r="AA11" s="0"/>
       <c r="AB11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1796,7 +1850,7 @@
       <c r="AA12" s="0"/>
       <c r="AB12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="4" t="s">
         <v>82</v>
       </c>
@@ -1864,7 +1918,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="4" t="s">
         <v>85</v>
       </c>
@@ -1932,7 +1986,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="4" t="s">
         <v>89</v>
       </c>
@@ -1982,7 +2036,7 @@
       <c r="AA15" s="0"/>
       <c r="AB15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="4" t="s">
         <v>94</v>
       </c>
@@ -2032,7 +2086,7 @@
       <c r="AA16" s="0"/>
       <c r="AB16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="4" t="s">
         <v>97</v>
       </c>
@@ -2080,7 +2134,7 @@
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="4" t="s">
         <v>99</v>
       </c>
@@ -2148,7 +2202,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="4" t="s">
         <v>104</v>
       </c>
@@ -2202,7 +2256,7 @@
       <c r="AA19" s="0"/>
       <c r="AB19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="4" t="s">
         <v>107</v>
       </c>
@@ -2270,7 +2324,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="4" t="s">
         <v>109</v>
       </c>
@@ -2318,7 +2372,7 @@
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="4" t="s">
         <v>116</v>
       </c>
@@ -2368,7 +2422,7 @@
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="4" t="s">
         <v>118</v>
       </c>
@@ -2436,7 +2490,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -2504,7 +2558,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="4" t="s">
         <v>124</v>
       </c>
@@ -2578,7 +2632,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="4" t="s">
         <v>107</v>
       </c>
@@ -2634,7 +2688,7 @@
       <c r="AA26" s="0"/>
       <c r="AB26" s="0"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="4" t="s">
         <v>130</v>
       </c>
@@ -2684,7 +2738,7 @@
       <c r="AA27" s="0"/>
       <c r="AB27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="4" t="s">
         <v>133</v>
       </c>
@@ -2744,7 +2798,7 @@
       <c r="AA28" s="0"/>
       <c r="AB28" s="0"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="A29" s="4" t="s">
         <v>135</v>
       </c>
@@ -2812,7 +2866,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="4" t="s">
         <v>137</v>
       </c>
@@ -2870,7 +2924,7 @@
       <c r="AA30" s="0"/>
       <c r="AB30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="A31" s="4" t="s">
         <v>139</v>
       </c>
@@ -2930,7 +2984,7 @@
       <c r="AA31" s="0"/>
       <c r="AB31" s="0"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="A32" s="4" t="s">
         <v>142</v>
       </c>
@@ -2997,7 +3051,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="4" t="s">
         <v>144</v>
       </c>
@@ -3044,7 +3098,7 @@
       <c r="AA33" s="0"/>
       <c r="AB33" s="0"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="4" t="s">
         <v>148</v>
       </c>
@@ -3111,7 +3165,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="4" t="s">
         <v>150</v>
       </c>
@@ -3178,7 +3232,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="4" t="s">
         <v>152</v>
       </c>
@@ -3245,7 +3299,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="4" t="s">
         <v>154</v>
       </c>
@@ -3308,7 +3362,7 @@
       <c r="AA37" s="0"/>
       <c r="AB37" s="0"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="4" t="s">
         <v>156</v>
       </c>
@@ -3375,7 +3429,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="4" t="s">
         <v>158</v>
       </c>
@@ -3432,7 +3486,7 @@
       <c r="AA39" s="0"/>
       <c r="AB39" s="0"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="4" t="s">
         <v>160</v>
       </c>
@@ -3479,7 +3533,7 @@
       <c r="AA40" s="0"/>
       <c r="AB40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="4" t="s">
         <v>162</v>
       </c>
@@ -3536,7 +3590,7 @@
       <c r="AA41" s="0"/>
       <c r="AB41" s="0"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="4" t="s">
         <v>165</v>
       </c>
@@ -3603,7 +3657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="4" t="s">
         <v>167</v>
       </c>
@@ -3670,7 +3724,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="4" t="s">
         <v>169</v>
       </c>
@@ -3727,7 +3781,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="4" t="s">
         <v>171</v>
       </c>
@@ -3794,7 +3848,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="4" t="s">
         <v>173</v>
       </c>
@@ -3847,7 +3901,7 @@
       <c r="AA46" s="0"/>
       <c r="AB46" s="0"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="4" t="s">
         <v>175</v>
       </c>
@@ -3904,7 +3958,7 @@
       <c r="AA47" s="0"/>
       <c r="AB47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="48">
       <c r="A48" s="4" t="s">
         <v>177</v>
       </c>
@@ -3961,7 +4015,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="49">
       <c r="A49" s="4" t="s">
         <v>179</v>
       </c>
@@ -4018,7 +4072,7 @@
       <c r="AA49" s="0"/>
       <c r="AB49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="A50" s="4" t="s">
         <v>181</v>
       </c>
@@ -4085,7 +4139,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="51">
       <c r="A51" s="4" t="s">
         <v>183</v>
       </c>
@@ -4152,7 +4206,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="52">
       <c r="A52" s="4" t="s">
         <v>139</v>
       </c>
@@ -4215,7 +4269,7 @@
       <c r="AA52" s="0"/>
       <c r="AB52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="A53" s="4" t="s">
         <v>187</v>
       </c>
@@ -4272,7 +4326,7 @@
       <c r="AA53" s="0"/>
       <c r="AB53" s="0"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="54">
       <c r="A54" s="4" t="s">
         <v>62</v>
       </c>
@@ -4339,7 +4393,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="55">
       <c r="A55" s="4" t="s">
         <v>190</v>
       </c>
@@ -4396,7 +4450,7 @@
       <c r="AA55" s="0"/>
       <c r="AB55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="56">
       <c r="A56" s="4" t="s">
         <v>191</v>
       </c>
@@ -4443,7 +4497,7 @@
       <c r="AA56" s="0"/>
       <c r="AB56" s="0"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="57">
       <c r="A57" s="4" t="s">
         <v>194</v>
       </c>
@@ -4510,7 +4564,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="58">
       <c r="A58" s="4" t="s">
         <v>197</v>
       </c>
@@ -4557,7 +4611,7 @@
       <c r="AA58" s="0"/>
       <c r="AB58" s="0"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="59">
       <c r="A59" s="4" t="s">
         <v>137</v>
       </c>
@@ -4624,7 +4678,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="60">
       <c r="A60" s="4" t="s">
         <v>201</v>
       </c>
@@ -4679,7 +4733,7 @@
       <c r="AA60" s="0"/>
       <c r="AB60" s="0"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="61">
       <c r="A61" s="4" t="s">
         <v>204</v>
       </c>
@@ -4746,7 +4800,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="62">
       <c r="A62" s="4" t="s">
         <v>206</v>
       </c>
@@ -4803,7 +4857,7 @@
       <c r="AA62" s="0"/>
       <c r="AB62" s="0"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="63">
       <c r="A63" s="4" t="s">
         <v>208</v>
       </c>
@@ -4870,7 +4924,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="64">
       <c r="A64" s="4" t="s">
         <v>210</v>
       </c>
@@ -4917,7 +4971,7 @@
       <c r="AA64" s="0"/>
       <c r="AB64" s="0"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="65">
       <c r="A65" s="4" t="s">
         <v>212</v>
       </c>
@@ -4984,7 +5038,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="66">
       <c r="A66" s="4" t="s">
         <v>214</v>
       </c>
@@ -5051,7 +5105,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="67">
       <c r="A67" s="4" t="s">
         <v>216</v>
       </c>
@@ -5108,7 +5162,7 @@
       <c r="AA67" s="0"/>
       <c r="AB67" s="0"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="68">
       <c r="A68" s="4" t="s">
         <v>62</v>
       </c>
@@ -5175,7 +5229,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="69">
       <c r="A69" s="4" t="s">
         <v>220</v>
       </c>
@@ -5222,7 +5276,7 @@
       <c r="AA69" s="0"/>
       <c r="AB69" s="0"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="70">
       <c r="A70" s="4" t="s">
         <v>222</v>
       </c>
@@ -5269,7 +5323,7 @@
       <c r="AA70" s="0"/>
       <c r="AB70" s="0"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="A71" s="4" t="s">
         <v>224</v>
       </c>
@@ -5342,7 +5396,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="72">
       <c r="A72" s="4" t="s">
         <v>226</v>
       </c>
@@ -5391,7 +5445,7 @@
       <c r="AA72" s="0"/>
       <c r="AB72" s="0"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="73">
       <c r="A73" s="4" t="s">
         <v>47</v>
       </c>
@@ -5458,7 +5512,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="74">
       <c r="A74" s="4" t="s">
         <v>232</v>
       </c>
@@ -5525,7 +5579,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="75">
       <c r="A75" s="4" t="s">
         <v>177</v>
       </c>
@@ -5592,7 +5646,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="76">
       <c r="A76" s="4" t="s">
         <v>82</v>
       </c>
@@ -5639,7 +5693,7 @@
       <c r="AA76" s="0"/>
       <c r="AB76" s="0"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="77">
       <c r="A77" s="4" t="s">
         <v>236</v>
       </c>
@@ -5686,7 +5740,7 @@
       <c r="AA77" s="0"/>
       <c r="AB77" s="0"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="78">
       <c r="A78" s="4" t="s">
         <v>238</v>
       </c>
@@ -5733,7 +5787,7 @@
       <c r="AA78" s="0"/>
       <c r="AB78" s="0"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="79">
       <c r="A79" s="4" t="s">
         <v>240</v>
       </c>
@@ -5780,7 +5834,7 @@
       <c r="AA79" s="0"/>
       <c r="AB79" s="0"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="80">
       <c r="A80" s="4" t="s">
         <v>62</v>
       </c>
@@ -5837,7 +5891,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="81">
       <c r="A81" s="4" t="s">
         <v>243</v>
       </c>
@@ -5904,7 +5958,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="82">
       <c r="A82" s="4" t="s">
         <v>244</v>
       </c>
@@ -5951,7 +6005,7 @@
       <c r="AA82" s="0"/>
       <c r="AB82" s="0"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="83">
       <c r="A83" s="4" t="s">
         <v>246</v>
       </c>
@@ -6014,7 +6068,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="84">
       <c r="A84" s="4" t="s">
         <v>248</v>
       </c>
@@ -6061,7 +6115,7 @@
       <c r="AA84" s="0"/>
       <c r="AB84" s="0"/>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="85">
       <c r="A85" s="4" t="s">
         <v>167</v>
       </c>
@@ -6118,7 +6172,7 @@
       <c r="AA85" s="0"/>
       <c r="AB85" s="0"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="86">
       <c r="A86" s="4" t="s">
         <v>252</v>
       </c>
@@ -6185,7 +6239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="87">
       <c r="A87" s="4" t="s">
         <v>254</v>
       </c>
@@ -6252,7 +6306,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="88">
       <c r="A88" s="4" t="s">
         <v>256</v>
       </c>
@@ -6304,7 +6358,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="89">
       <c r="A89" s="4" t="s">
         <v>258</v>
       </c>
@@ -6356,7 +6410,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="90">
       <c r="A90" s="4" t="s">
         <v>260</v>
       </c>
@@ -6398,7 +6452,7 @@
       <c r="AA90" s="0"/>
       <c r="AB90" s="0"/>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="91">
       <c r="A91" s="4" t="s">
         <v>204</v>
       </c>
@@ -6450,7 +6504,7 @@
       <c r="AA91" s="0"/>
       <c r="AB91" s="0"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="92">
       <c r="A92" s="4" t="s">
         <v>264</v>
       </c>
@@ -6502,7 +6556,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="93">
       <c r="A93" s="4" t="s">
         <v>266</v>
       </c>
@@ -6554,7 +6608,7 @@
       <c r="AA93" s="0"/>
       <c r="AB93" s="0"/>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="94">
       <c r="A94" s="4" t="s">
         <v>25</v>
       </c>
@@ -6601,7 +6655,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="95">
       <c r="A95" s="4" t="s">
         <v>269</v>
       </c>
@@ -6638,7 +6692,7 @@
       <c r="AA95" s="0"/>
       <c r="AB95" s="0"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="96">
       <c r="A96" s="4" t="s">
         <v>271</v>
       </c>
@@ -6685,7 +6739,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="97">
       <c r="A97" s="4" t="s">
         <v>273</v>
       </c>
@@ -6732,7 +6786,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="98">
       <c r="A98" s="4" t="s">
         <v>275</v>
       </c>
@@ -6764,7 +6818,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="99">
       <c r="A99" s="4" t="s">
         <v>177</v>
       </c>
@@ -6797,9 +6851,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6814,23 +6868,23 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="A17" activeCellId="0" pane="topLeft" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.0407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.87777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.2037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.8666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36296296296296"/>
+    <col min="1" max="1" hidden="false" style="0" width="52.0407407407407" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="9.87777777777778" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="9.2037037037037" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="13.7111111111111" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="18.7555555555556" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="10.6222222222222" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="15.8666666666667" collapsed="true"/>
+    <col min="8" max="1025" hidden="false" style="0" width="8.36296296296296" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>278</v>
       </c>
@@ -6844,7 +6898,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="B2" s="0" t="s">
         <v>282</v>
       </c>
@@ -6858,7 +6912,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>286</v>
       </c>
@@ -6878,7 +6932,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>58</v>
       </c>
@@ -6904,7 +6958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>37</v>
       </c>
@@ -6930,7 +6984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>288</v>
       </c>
@@ -6956,7 +7010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>44</v>
       </c>
@@ -6982,7 +7036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>291</v>
       </c>
@@ -7008,7 +7062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>81</v>
       </c>
@@ -7034,7 +7088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>293</v>
       </c>
@@ -7048,7 +7102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>295</v>
       </c>
@@ -7062,7 +7116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>296</v>
       </c>
@@ -7076,7 +7130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>59</v>
       </c>
@@ -7102,7 +7156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>297</v>
       </c>
@@ -7116,55 +7170,55 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>306</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.025" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.025"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>

</xml_diff>